<commit_message>
bugs in printout file fixed
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t>Conventional generation (MW)</t>
   </si>
@@ -37,9 +37,6 @@
     <t>angle(degs)</t>
   </si>
   <si>
-    <t>Voltage(p.u.)</t>
-  </si>
-  <si>
     <t>busname</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>alpha</t>
   </si>
   <si>
-    <t>QD(MW)</t>
-  </si>
-  <si>
     <t>D14</t>
   </si>
   <si>
@@ -103,16 +97,109 @@
     <t>D1</t>
   </si>
   <si>
-    <t>PGLB(MW)</t>
+    <t>PG(MW)</t>
   </si>
   <si>
     <t>pG(MW)</t>
   </si>
   <si>
-    <t>PGUB(MW)</t>
-  </si>
-  <si>
-    <t>('QGLB(MW)', 'qG(MW)', 'QGUB(MW)')</t>
+    <t>G19</t>
+  </si>
+  <si>
+    <t>G16</t>
+  </si>
+  <si>
+    <t>G24</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G13</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G28</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G17</t>
+  </si>
+  <si>
+    <t>G23</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G14</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>G31</t>
+  </si>
+  <si>
+    <t>G30</t>
+  </si>
+  <si>
+    <t>G25</t>
+  </si>
+  <si>
+    <t>G22</t>
+  </si>
+  <si>
+    <t>G29</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G15</t>
+  </si>
+  <si>
+    <t>G21</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G26</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G18</t>
+  </si>
+  <si>
+    <t>G32</t>
+  </si>
+  <si>
+    <t>G33</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G20</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>G27</t>
   </si>
   <si>
     <t>PW(MW)</t>
@@ -127,13 +214,7 @@
     <t>to_busname</t>
   </si>
   <si>
-    <t>pLto(MW)</t>
-  </si>
-  <si>
-    <t>pLfrom(MW)</t>
-  </si>
-  <si>
-    <t>loss(MW)</t>
+    <t>pL(MW)</t>
   </si>
   <si>
     <t>L16-1223</t>
@@ -235,10 +316,7 @@
     <t>L28-1821</t>
   </si>
   <si>
-    <t>pLTto(MW)</t>
-  </si>
-  <si>
-    <t>pLTfrom(MW)</t>
+    <t>pLT(MW)</t>
   </si>
   <si>
     <t>T2-911</t>
@@ -630,7 +708,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2896.765548072822</v>
+        <v>2850.000028498449</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -646,285 +724,210 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-6.755434884756172</v>
-      </c>
-      <c r="C2">
-        <v>1.047227547524992</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>9.242226441113573</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-6.831083490839968</v>
-      </c>
-      <c r="C3">
-        <v>1.047206283621973</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>8.457026648178182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-6.187465633641493</v>
-      </c>
-      <c r="C4">
-        <v>1.013779184867813</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>41.15829541210107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-9.574331497091887</v>
-      </c>
-      <c r="C5">
-        <v>1.01624866058875</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>7.409010687426385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-9.737554712491487</v>
-      </c>
-      <c r="C6">
-        <v>1.035427233010197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>-1.85244231717763</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-12.31054826145475</v>
-      </c>
-      <c r="C7">
-        <v>1.032406020324406</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>-9.05133702463624</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-9.876561561749863</v>
-      </c>
-      <c r="C8">
-        <v>1.036004572887004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>1.943989160966431</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-12.5531651414247</v>
-      </c>
-      <c r="C9">
-        <v>1.008963398698759</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>-2.101665789242874</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-7.818243368184379</v>
-      </c>
-      <c r="C10">
-        <v>1.023926693435027</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>10.94800586874138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-9.678324589918676</v>
-      </c>
-      <c r="C11">
-        <v>1.050000004431561</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>-9.853998583977292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-2.613089336661063</v>
-      </c>
-      <c r="C12">
-        <v>1.022627010851432</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>11.83628175767672</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-1.876066036690312</v>
-      </c>
-      <c r="C13">
-        <v>1.017272788512978</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>-10.52563997905581</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>3.675190887696723e-30</v>
-      </c>
-      <c r="C14">
-        <v>1.033477333202541</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>-9.17527102641913e-29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1.012438740529386</v>
-      </c>
-      <c r="C15">
-        <v>1.039865131773935</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>3.371765297953462</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>9.324357506537345</v>
-      </c>
-      <c r="C16">
-        <v>1.041060688957348</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>-4.386200130258183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>8.542574724883009</v>
-      </c>
-      <c r="C17">
-        <v>1.044277246263287</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>-0.1816171205750362</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>12.89163330956417</v>
-      </c>
-      <c r="C18">
-        <v>1.047564196049829</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>2.821184219290648</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>14.2470368563342</v>
-      </c>
-      <c r="C19">
-        <v>1.049999985615682</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>3.461413518871765</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>7.493157871532119</v>
-      </c>
-      <c r="C20">
-        <v>1.038946882103307</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>-0.08362842811170122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>8.452298138845665</v>
-      </c>
-      <c r="C21">
-        <v>1.043973888312215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>2.053728046438543</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>15.02296051882872</v>
-      </c>
-      <c r="C22">
-        <v>1.050000002300528</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>3.540048478194987</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>20.69119238604117</v>
-      </c>
-      <c r="C23">
-        <v>1.049999996772942</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>10.34780789419934</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>9.683768873834786</v>
-      </c>
-      <c r="C24">
-        <v>1.049999999094497</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>4.011615714646209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>3.668279519969537</v>
-      </c>
-      <c r="C25">
-        <v>1.005845487048798</v>
+        <v>-30.75753130153424</v>
       </c>
     </row>
   </sheetData>
@@ -934,32 +937,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -970,13 +970,10 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>19</v>
@@ -987,13 +984,10 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1004,13 +998,10 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -1021,13 +1012,10 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1038,13 +1026,10 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -1055,13 +1040,10 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1072,13 +1054,10 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -1089,13 +1068,10 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1106,13 +1082,10 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>13</v>
@@ -1123,13 +1096,10 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>20</v>
@@ -1140,13 +1110,10 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1157,13 +1124,10 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1174,13 +1138,10 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -1191,13 +1152,10 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -1208,13 +1166,10 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>18</v>
@@ -1225,13 +1180,10 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1241,9 +1193,6 @@
       </c>
       <c r="D18">
         <v>1</v>
-      </c>
-      <c r="E18">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1253,30 +1202,486 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2">
+        <v>0.12</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C3">
+        <v>0.12</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
+      </c>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>0.951</v>
+      </c>
+      <c r="D6">
+        <v>45.333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>0.8</v>
+      </c>
+      <c r="D7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>0.8</v>
+      </c>
+      <c r="D10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11">
+        <v>0.12</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>0.76</v>
+      </c>
+      <c r="D13">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>0.951</v>
+      </c>
+      <c r="D14">
+        <v>45.333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>0.8</v>
+      </c>
+      <c r="D15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>1.55</v>
+      </c>
+      <c r="D16">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19">
+        <v>1.55</v>
+      </c>
+      <c r="D19">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>0.76</v>
+      </c>
+      <c r="D21">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>1.55</v>
+      </c>
+      <c r="D23">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24">
+        <v>0.76</v>
+      </c>
+      <c r="D24">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="D25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26">
+        <v>0.76</v>
+      </c>
+      <c r="D26">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27">
+        <v>0.12</v>
+      </c>
+      <c r="D27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28">
+        <v>1.55</v>
+      </c>
+      <c r="D28">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29">
+        <v>3.5</v>
+      </c>
+      <c r="D29">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30">
+        <v>0.1</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31">
+        <v>0.12</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32">
+        <v>0.1</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33">
+        <v>0.951</v>
+      </c>
+      <c r="D33">
+        <v>45.333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1297,13 +1702,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1313,35 +1718,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1350,18 +1749,12 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <v>225.3116000465253</v>
-      </c>
-      <c r="E2">
-        <v>-219.506831114251</v>
-      </c>
-      <c r="F2">
-        <v>5.804768932274351</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>-262.6531843263409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1370,18 +1763,12 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>-51.69920766795152</v>
-      </c>
-      <c r="E3">
-        <v>52.97533190169651</v>
-      </c>
-      <c r="F3">
-        <v>1.276124233744991</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>159.1555170453038</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -1390,18 +1777,12 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>180.3504799766482</v>
-      </c>
-      <c r="E4">
-        <v>-179.8193241260269</v>
-      </c>
-      <c r="F4">
-        <v>0.5311558506213121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>-77.59798087097556</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -1410,18 +1791,12 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>159.0093346406055</v>
-      </c>
-      <c r="E5">
-        <v>-157.001899744802</v>
-      </c>
-      <c r="F5">
-        <v>2.007434895803417</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>-175.2475169515317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -1430,18 +1805,12 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>364.42033172087</v>
-      </c>
-      <c r="E6">
-        <v>-358.3258957059193</v>
-      </c>
-      <c r="F6">
-        <v>6.094436014950677</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>159.4298786265158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1450,18 +1819,12 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>-84.83779465758819</v>
-      </c>
-      <c r="E7">
-        <v>86.02828470508793</v>
-      </c>
-      <c r="F7">
-        <v>1.190490047499737</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>114.9999988283158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1470,18 +1833,12 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>-21.06213426257768</v>
-      </c>
-      <c r="E8">
-        <v>21.25452953088823</v>
-      </c>
-      <c r="F8">
-        <v>0.1923952683105523</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>443.0832105147713</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -1490,18 +1847,12 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>318.3715245403725</v>
-      </c>
-      <c r="E9">
-        <v>-315.316617590942</v>
-      </c>
-      <c r="F9">
-        <v>3.054906949430514</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>-202.3504639532859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1510,18 +1861,12 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>30.7756131875831</v>
-      </c>
-      <c r="E10">
-        <v>-30.53350193137052</v>
-      </c>
-      <c r="F10">
-        <v>0.2421112562125904</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>-59.5632768815294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>15</v>
@@ -1530,18 +1875,12 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <v>-203.0098915284346</v>
-      </c>
-      <c r="E11">
-        <v>205.8079035306464</v>
-      </c>
-      <c r="F11">
-        <v>2.798012002211747</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>886.8334432983494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1550,18 +1889,12 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <v>164.3258947522075</v>
-      </c>
-      <c r="E12">
-        <v>-162.9416677873203</v>
-      </c>
-      <c r="F12">
-        <v>1.384226964887181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>353.4298607932289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -1570,18 +1903,12 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>102.8517877684069</v>
-      </c>
-      <c r="E13">
-        <v>-102.2384369151303</v>
-      </c>
-      <c r="F13">
-        <v>0.6133508532766285</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>433.9959829091649</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1590,18 +1917,12 @@
         <v>23</v>
       </c>
       <c r="D14">
-        <v>212.3914039015858</v>
-      </c>
-      <c r="E14">
-        <v>-207.8382287811901</v>
-      </c>
-      <c r="F14">
-        <v>4.553175120395681</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>-80.94323993665854</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -1610,18 +1931,12 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>111.1485009062116</v>
-      </c>
-      <c r="E15">
-        <v>-110.8282003144748</v>
-      </c>
-      <c r="F15">
-        <v>0.320300591736844</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>-158.2017879371334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1630,18 +1945,12 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <v>-81.87489113923536</v>
-      </c>
-      <c r="E16">
-        <v>82.02878694805689</v>
-      </c>
-      <c r="F16">
-        <v>0.1538958088215248</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>-424.1839144068965</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -1650,18 +1959,12 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>140.9906701536435</v>
-      </c>
-      <c r="E17">
-        <v>-138.5522004143456</v>
-      </c>
-      <c r="F17">
-        <v>2.438469739297844</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>-124.7524830823103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1670,18 +1973,12 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>0.7860716544951287</v>
-      </c>
-      <c r="E18">
-        <v>-0.6457334086400762</v>
-      </c>
-      <c r="F18">
-        <v>0.1403382458550526</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>-263.7502309836688</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -1690,18 +1987,12 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>56.77311781627225</v>
-      </c>
-      <c r="E19">
-        <v>-56.67523976155107</v>
-      </c>
-      <c r="F19">
-        <v>0.09787805472118993</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>-5.298992074751678</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -1710,18 +2001,12 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>51.18156226472655</v>
-      </c>
-      <c r="E20">
-        <v>-50.11332675127505</v>
-      </c>
-      <c r="F20">
-        <v>1.06823551345151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>-137.9525964481421</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -1730,18 +2015,12 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>221.7278339474302</v>
-      </c>
-      <c r="E21">
-        <v>-218.9183465233798</v>
-      </c>
-      <c r="F21">
-        <v>2.809487424050428</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>-282.3247664267045</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -1750,18 +2029,12 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <v>85.23759245409964</v>
-      </c>
-      <c r="E22">
-        <v>-84.30079369195752</v>
-      </c>
-      <c r="F22">
-        <v>0.9367987621421214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>23.15551568539471</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1770,18 +2043,12 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>-43.46649880853853</v>
-      </c>
-      <c r="E23">
-        <v>44.11708992827864</v>
-      </c>
-      <c r="F23">
-        <v>0.6505911197401126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>14.43672385837969</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1790,18 +2057,12 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>-10.09242315308474</v>
-      </c>
-      <c r="E24">
-        <v>10.09490938155504</v>
-      </c>
-      <c r="F24">
-        <v>0.002486228470299778</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>98.5922422496897</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="B25">
         <v>19</v>
@@ -1810,18 +2071,12 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>46.82819967452027</v>
-      </c>
-      <c r="E25">
-        <v>-46.72287908882835</v>
-      </c>
-      <c r="F25">
-        <v>0.1053205856919204</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>-94.20178729717887</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="B26">
         <v>20</v>
@@ -1830,18 +2085,12 @@
         <v>23</v>
       </c>
       <c r="D26">
-        <v>111.1485009062116</v>
-      </c>
-      <c r="E26">
-        <v>-110.8282003144748</v>
-      </c>
-      <c r="F26">
-        <v>0.320300591736844</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>-158.2017879371334</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1850,18 +2099,12 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <v>-65.67029063988511</v>
-      </c>
-      <c r="E27">
-        <v>66.5508225934507</v>
-      </c>
-      <c r="F27">
-        <v>0.8805319535655887</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>229.1579872779728</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -1870,18 +2113,12 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>-87.55424363225234</v>
-      </c>
-      <c r="E28">
-        <v>87.77117728249596</v>
-      </c>
-      <c r="F28">
-        <v>0.2169336502436225</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>-7.403572784448646</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -1890,18 +2127,12 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>36.68767643258914</v>
-      </c>
-      <c r="E29">
-        <v>-36.04888030104579</v>
-      </c>
-      <c r="F29">
-        <v>0.638796131543351</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>81.95259356654881</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="B30">
         <v>12</v>
@@ -1910,18 +2141,12 @@
         <v>13</v>
       </c>
       <c r="D30">
-        <v>75.72368020563626</v>
-      </c>
-      <c r="E30">
-        <v>-75.35559446873461</v>
-      </c>
-      <c r="F30">
-        <v>0.3680857369016466</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>-385.9392300707591</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -1930,18 +2155,12 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>5.38824782838519</v>
-      </c>
-      <c r="E31">
-        <v>-5.329710070023923</v>
-      </c>
-      <c r="F31">
-        <v>0.05853775836126771</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>158.1579865680637</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B32">
         <v>19</v>
@@ -1950,18 +2169,12 @@
         <v>20</v>
       </c>
       <c r="D32">
-        <v>46.82819967452027</v>
-      </c>
-      <c r="E32">
-        <v>-46.72287908882835</v>
-      </c>
-      <c r="F32">
-        <v>0.1053205856919204</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>-94.20178729717887</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="B33">
         <v>15</v>
@@ -1970,18 +2183,12 @@
         <v>21</v>
       </c>
       <c r="D33">
-        <v>221.7278339474302</v>
-      </c>
-      <c r="E33">
-        <v>-218.9183465233798</v>
-      </c>
-      <c r="F33">
-        <v>2.809487424050428</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>-282.3247664267045</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="B34">
         <v>18</v>
@@ -1990,13 +2197,7 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>56.77311781627225</v>
-      </c>
-      <c r="E34">
-        <v>-56.67523976155107</v>
-      </c>
-      <c r="F34">
-        <v>0.09787805472118993</v>
+        <v>-5.298992074751665</v>
       </c>
     </row>
   </sheetData>
@@ -2006,35 +2207,29 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -2043,18 +2238,12 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>110.9326547858927</v>
-      </c>
-      <c r="E2">
-        <v>-110.6323443040448</v>
-      </c>
-      <c r="F2">
-        <v>0.3003104818478874</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>53916.26102081346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -2063,18 +2252,12 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>125.6350414727596</v>
-      </c>
-      <c r="E3">
-        <v>-125.2626986355961</v>
-      </c>
-      <c r="F3">
-        <v>0.372342837163453</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>-53845.69368537825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -2083,18 +2266,12 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>154.2474499165578</v>
-      </c>
-      <c r="E4">
-        <v>-153.7239816305747</v>
-      </c>
-      <c r="F4">
-        <v>0.523468285983153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>-53128.83517711105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2103,18 +2280,12 @@
         <v>24</v>
       </c>
       <c r="D5">
-        <v>203.0098915284346</v>
-      </c>
-      <c r="E5">
-        <v>-202.0406029852924</v>
-      </c>
-      <c r="F5">
-        <v>0.9692885431422216</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>-886.8334432983494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -2123,13 +2294,7 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>169.227384110226</v>
-      </c>
-      <c r="E6">
-        <v>-168.5895370344083</v>
-      </c>
-      <c r="F6">
-        <v>0.6378470758176658</v>
+        <v>53197.10127098116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UC model added to the the models library.
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="111">
   <si>
     <t>Conventional generation (MW)</t>
   </si>
@@ -37,6 +37,9 @@
     <t>angle(degs)</t>
   </si>
   <si>
+    <t>Voltage(p.u.)</t>
+  </si>
+  <si>
     <t>busname</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t>alpha</t>
   </si>
   <si>
+    <t>QD(MVar)</t>
+  </si>
+  <si>
     <t>D14</t>
   </si>
   <si>
@@ -97,12 +103,24 @@
     <t>D1</t>
   </si>
   <si>
-    <t>PG(MW)</t>
+    <t>PGLB(MW)</t>
   </si>
   <si>
     <t>pG(MW)</t>
   </si>
   <si>
+    <t>PGUB(MW)</t>
+  </si>
+  <si>
+    <t>QGLB(MVar)</t>
+  </si>
+  <si>
+    <t>qG(MVar)</t>
+  </si>
+  <si>
+    <t>QGUB(MVar)</t>
+  </si>
+  <si>
     <t>G19</t>
   </si>
   <si>
@@ -202,19 +220,19 @@
     <t>G27</t>
   </si>
   <si>
-    <t>PW(MW)</t>
-  </si>
-  <si>
-    <t>pW(MW)</t>
-  </si>
-  <si>
     <t>from_busname</t>
   </si>
   <si>
     <t>to_busname</t>
   </si>
   <si>
-    <t>pL(MW)</t>
+    <t>pLto(MW)</t>
+  </si>
+  <si>
+    <t>pLfrom(MW)</t>
+  </si>
+  <si>
+    <t>loss(MW)</t>
   </si>
   <si>
     <t>L16-1223</t>
@@ -316,7 +334,10 @@
     <t>L28-1821</t>
   </si>
   <si>
-    <t>pLT(MW)</t>
+    <t>pLTto(MW)</t>
+  </si>
+  <si>
+    <t>pLTfrom(MW)</t>
   </si>
   <si>
     <t>T2-911</t>
@@ -708,7 +729,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2850.000028498449</v>
+        <v>2896.765548072822</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -724,210 +745,285 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9.242226441113573</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>-6.755434884756172</v>
+      </c>
+      <c r="C2">
+        <v>1.047227547524992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>8.457026648178182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>-6.831083490839968</v>
+      </c>
+      <c r="C3">
+        <v>1.047206283621973</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>41.15829541210107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>-6.187465633641493</v>
+      </c>
+      <c r="C4">
+        <v>1.013779184867813</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7.409010687426385</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>-9.574331497091887</v>
+      </c>
+      <c r="C5">
+        <v>1.01624866058875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-1.85244231717763</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>-9.737554712491487</v>
+      </c>
+      <c r="C6">
+        <v>1.035427233010197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-9.05133702463624</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>-12.31054826145475</v>
+      </c>
+      <c r="C7">
+        <v>1.032406020324406</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1.943989160966431</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>-9.876561561749863</v>
+      </c>
+      <c r="C8">
+        <v>1.036004572887004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-2.101665789242874</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>-12.5531651414247</v>
+      </c>
+      <c r="C9">
+        <v>1.008963398698759</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>10.94800586874138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>-7.818243368184379</v>
+      </c>
+      <c r="C10">
+        <v>1.023926693435027</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-9.853998583977292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>-9.678324589918676</v>
+      </c>
+      <c r="C11">
+        <v>1.050000004431561</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>11.83628175767672</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>-2.613089336661063</v>
+      </c>
+      <c r="C12">
+        <v>1.022627010851432</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-10.52563997905581</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>-1.876066036690312</v>
+      </c>
+      <c r="C13">
+        <v>1.017272788512978</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-9.17527102641913e-29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>3.675190887696723e-30</v>
+      </c>
+      <c r="C14">
+        <v>1.033477333202541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>3.371765297953462</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>1.012438740529386</v>
+      </c>
+      <c r="C15">
+        <v>1.039865131773935</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-4.386200130258183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>9.324357506537345</v>
+      </c>
+      <c r="C16">
+        <v>1.041060688957348</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>-0.1816171205750362</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>8.542574724883009</v>
+      </c>
+      <c r="C17">
+        <v>1.044277246263287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>2.821184219290648</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>12.89163330956417</v>
+      </c>
+      <c r="C18">
+        <v>1.047564196049829</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>3.461413518871765</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>14.2470368563342</v>
+      </c>
+      <c r="C19">
+        <v>1.049999985615682</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>-0.08362842811170122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>7.493157871532119</v>
+      </c>
+      <c r="C20">
+        <v>1.038946882103307</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>2.053728046438543</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>8.452298138845665</v>
+      </c>
+      <c r="C21">
+        <v>1.043973888312215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>3.540048478194987</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>15.02296051882872</v>
+      </c>
+      <c r="C22">
+        <v>1.050000002300528</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>10.34780789419934</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>20.69119238604117</v>
+      </c>
+      <c r="C23">
+        <v>1.049999996772942</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>4.011615714646209</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>9.683768873834786</v>
+      </c>
+      <c r="C24">
+        <v>1.049999999094497</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-30.75753130153424</v>
+        <v>3.668279519969537</v>
+      </c>
+      <c r="C25">
+        <v>1.005845487048798</v>
       </c>
     </row>
   </sheetData>
@@ -937,29 +1033,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -970,10 +1069,13 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>19</v>
@@ -984,10 +1086,13 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -998,10 +1103,13 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -1012,10 +1120,13 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1026,10 +1137,13 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -1040,10 +1154,13 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1054,10 +1171,13 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -1068,10 +1188,13 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1082,10 +1205,13 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>13</v>
@@ -1096,10 +1222,13 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>20</v>
@@ -1110,10 +1239,13 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1124,10 +1256,13 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1138,10 +1273,13 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -1152,10 +1290,13 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -1166,10 +1307,13 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>18</v>
@@ -1180,10 +1324,13 @@
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1193,6 +1340,9 @@
       </c>
       <c r="D18">
         <v>1</v>
+      </c>
+      <c r="E18">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1202,312 +1352,564 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C2">
-        <v>0.12</v>
+        <v>2.4</v>
       </c>
       <c r="D2">
+        <v>2.4</v>
+      </c>
+      <c r="E2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C3">
-        <v>0.12</v>
+        <v>2.4</v>
       </c>
       <c r="D3">
+        <v>2.4</v>
+      </c>
+      <c r="E3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="D4">
         <v>400</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>400</v>
+      </c>
+      <c r="F4">
+        <v>-50</v>
+      </c>
+      <c r="G4">
+        <v>-7.458</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>16</v>
       </c>
       <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>4.862</v>
+      </c>
+      <c r="H5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C6">
-        <v>0.951</v>
+        <v>69</v>
       </c>
       <c r="D6">
-        <v>45.333</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>78.57899999999999</v>
+      </c>
+      <c r="E6">
+        <v>197</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>32.592</v>
+      </c>
+      <c r="H6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <v>0.8</v>
+        <v>25</v>
       </c>
       <c r="D7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>70.343</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>16.438</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>16</v>
       </c>
       <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>4.814</v>
+      </c>
+      <c r="H8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>-10</v>
+      </c>
+      <c r="G9">
+        <v>-6.413</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C10">
-        <v>0.8</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>70.343</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>16.438</v>
+      </c>
+      <c r="H10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C11">
-        <v>0.12</v>
+        <v>2.4</v>
       </c>
       <c r="D11">
+        <v>2.4</v>
+      </c>
+      <c r="E11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="D12">
         <v>400</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>400</v>
+      </c>
+      <c r="F12">
+        <v>-50</v>
+      </c>
+      <c r="G12">
+        <v>72.898</v>
+      </c>
+      <c r="H12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C13">
-        <v>0.76</v>
+        <v>15.2</v>
       </c>
       <c r="D13">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>76</v>
+      </c>
+      <c r="F13">
+        <v>-25</v>
+      </c>
+      <c r="G13">
+        <v>-1.576</v>
+      </c>
+      <c r="H13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>0.951</v>
+        <v>69</v>
       </c>
       <c r="D14">
-        <v>45.333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>78.57899999999999</v>
+      </c>
+      <c r="E14">
+        <v>197</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>32.592</v>
+      </c>
+      <c r="H14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C15">
-        <v>0.8</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>70.343</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>16.438</v>
+      </c>
+      <c r="H15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C16">
-        <v>1.55</v>
+        <v>54.3</v>
       </c>
       <c r="D16">
         <v>155</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>155</v>
+      </c>
+      <c r="F16">
+        <v>-50</v>
+      </c>
+      <c r="G16">
+        <v>2.547</v>
+      </c>
+      <c r="H16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C17">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>50</v>
+      </c>
+      <c r="F17">
+        <v>-10</v>
+      </c>
+      <c r="G17">
+        <v>-6.413</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>50</v>
+      </c>
+      <c r="F18">
+        <v>-10</v>
+      </c>
+      <c r="G18">
+        <v>-6.413</v>
+      </c>
+      <c r="H18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C19">
-        <v>1.55</v>
+        <v>54.3</v>
       </c>
       <c r="D19">
         <v>155</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>155</v>
+      </c>
+      <c r="F19">
+        <v>-50</v>
+      </c>
+      <c r="G19">
+        <v>80</v>
+      </c>
+      <c r="H19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C20">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D20">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>50</v>
+      </c>
+      <c r="F20">
+        <v>-10</v>
+      </c>
+      <c r="G20">
+        <v>-6.413</v>
+      </c>
+      <c r="H20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C21">
-        <v>0.76</v>
+        <v>15.2</v>
       </c>
       <c r="D21">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>76</v>
+      </c>
+      <c r="F21">
+        <v>-25</v>
+      </c>
+      <c r="G21">
+        <v>-2.923</v>
+      </c>
+      <c r="H21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1515,173 +1917,329 @@
       <c r="D22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>-50</v>
+      </c>
+      <c r="G22">
+        <v>114.908</v>
+      </c>
+      <c r="H22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C23">
-        <v>1.55</v>
+        <v>54.3</v>
       </c>
       <c r="D23">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>155</v>
+      </c>
+      <c r="F23">
+        <v>-50</v>
+      </c>
+      <c r="G23">
+        <v>80</v>
+      </c>
+      <c r="H23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C24">
-        <v>0.76</v>
+        <v>15.2</v>
       </c>
       <c r="D24">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>76</v>
+      </c>
+      <c r="F24">
+        <v>-25</v>
+      </c>
+      <c r="G24">
+        <v>-2.923</v>
+      </c>
+      <c r="H24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C25">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D25">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>50</v>
+      </c>
+      <c r="F25">
+        <v>-10</v>
+      </c>
+      <c r="G25">
+        <v>-6.413</v>
+      </c>
+      <c r="H25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C26">
-        <v>0.76</v>
+        <v>15.2</v>
       </c>
       <c r="D26">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>76</v>
+      </c>
+      <c r="F26">
+        <v>-25</v>
+      </c>
+      <c r="G26">
+        <v>-1.576</v>
+      </c>
+      <c r="H26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C27">
-        <v>0.12</v>
+        <v>2.4</v>
       </c>
       <c r="D27">
+        <v>2.4</v>
+      </c>
+      <c r="E27">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C28">
-        <v>1.55</v>
+        <v>54.3</v>
       </c>
       <c r="D28">
         <v>155</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>155</v>
+      </c>
+      <c r="F28">
+        <v>-50</v>
+      </c>
+      <c r="G28">
+        <v>2.547</v>
+      </c>
+      <c r="H28">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C29">
-        <v>3.5</v>
+        <v>140</v>
       </c>
       <c r="D29">
         <v>350</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>350</v>
+      </c>
+      <c r="F29">
+        <v>-25</v>
+      </c>
+      <c r="G29">
+        <v>40.549</v>
+      </c>
+      <c r="H29">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C30">
-        <v>0.1</v>
+        <v>16</v>
       </c>
       <c r="D30">
+        <v>16</v>
+      </c>
+      <c r="E30">
+        <v>20</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>4.814</v>
+      </c>
+      <c r="H30">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C31">
-        <v>0.12</v>
+        <v>2.4</v>
       </c>
       <c r="D31">
+        <v>2.4</v>
+      </c>
+      <c r="E31">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C32">
-        <v>0.1</v>
+        <v>16</v>
       </c>
       <c r="D32">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>4.862</v>
+      </c>
+      <c r="H32">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C33">
-        <v>0.951</v>
+        <v>69</v>
       </c>
       <c r="D33">
-        <v>45.333</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>78.57899999999999</v>
+      </c>
+      <c r="E33">
+        <v>197</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>32.592</v>
+      </c>
+      <c r="H33">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C34">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D34">
         <v>50</v>
+      </c>
+      <c r="E34">
+        <v>50</v>
+      </c>
+      <c r="F34">
+        <v>-10</v>
+      </c>
+      <c r="G34">
+        <v>-6.413</v>
+      </c>
+      <c r="H34">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1691,24 +2249,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1718,29 +2288,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1749,12 +2325,18 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <v>-262.6531843263409</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>225.3116000465253</v>
+      </c>
+      <c r="E2">
+        <v>-219.506831114251</v>
+      </c>
+      <c r="F2">
+        <v>5.804768932274351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1763,12 +2345,18 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>159.1555170453038</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>-51.69920766795152</v>
+      </c>
+      <c r="E3">
+        <v>52.97533190169651</v>
+      </c>
+      <c r="F3">
+        <v>1.276124233744991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -1777,12 +2365,18 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>-77.59798087097556</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>180.3504799766482</v>
+      </c>
+      <c r="E4">
+        <v>-179.8193241260269</v>
+      </c>
+      <c r="F4">
+        <v>0.5311558506213121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -1791,12 +2385,18 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>-175.2475169515317</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>159.0093346406055</v>
+      </c>
+      <c r="E5">
+        <v>-157.001899744802</v>
+      </c>
+      <c r="F5">
+        <v>2.007434895803417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -1805,12 +2405,18 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>159.4298786265158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>364.42033172087</v>
+      </c>
+      <c r="E6">
+        <v>-358.3258957059193</v>
+      </c>
+      <c r="F6">
+        <v>6.094436014950677</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1819,12 +2425,18 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>114.9999988283158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>-84.83779465758819</v>
+      </c>
+      <c r="E7">
+        <v>86.02828470508793</v>
+      </c>
+      <c r="F7">
+        <v>1.190490047499737</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1833,12 +2445,18 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>443.0832105147713</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>-21.06213426257768</v>
+      </c>
+      <c r="E8">
+        <v>21.25452953088823</v>
+      </c>
+      <c r="F8">
+        <v>0.1923952683105523</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -1847,12 +2465,18 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>-202.3504639532859</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>318.3715245403725</v>
+      </c>
+      <c r="E9">
+        <v>-315.316617590942</v>
+      </c>
+      <c r="F9">
+        <v>3.054906949430514</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1861,12 +2485,18 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>-59.5632768815294</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>30.7756131875831</v>
+      </c>
+      <c r="E10">
+        <v>-30.53350193137052</v>
+      </c>
+      <c r="F10">
+        <v>0.2421112562125904</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B11">
         <v>15</v>
@@ -1875,12 +2505,18 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <v>886.8334432983494</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>-203.0098915284346</v>
+      </c>
+      <c r="E11">
+        <v>205.8079035306464</v>
+      </c>
+      <c r="F11">
+        <v>2.798012002211747</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1889,12 +2525,18 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <v>353.4298607932289</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>164.3258947522075</v>
+      </c>
+      <c r="E12">
+        <v>-162.9416677873203</v>
+      </c>
+      <c r="F12">
+        <v>1.384226964887181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -1903,12 +2545,18 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>433.9959829091649</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>102.8517877684069</v>
+      </c>
+      <c r="E13">
+        <v>-102.2384369151303</v>
+      </c>
+      <c r="F13">
+        <v>0.6133508532766285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1917,12 +2565,18 @@
         <v>23</v>
       </c>
       <c r="D14">
-        <v>-80.94323993665854</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>212.3914039015858</v>
+      </c>
+      <c r="E14">
+        <v>-207.8382287811901</v>
+      </c>
+      <c r="F14">
+        <v>4.553175120395681</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -1931,12 +2585,18 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>-158.2017879371334</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>111.1485009062116</v>
+      </c>
+      <c r="E15">
+        <v>-110.8282003144748</v>
+      </c>
+      <c r="F15">
+        <v>0.320300591736844</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1945,12 +2605,18 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <v>-424.1839144068965</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>-81.87489113923536</v>
+      </c>
+      <c r="E16">
+        <v>82.02878694805689</v>
+      </c>
+      <c r="F16">
+        <v>0.1538958088215248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -1959,12 +2625,18 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>-124.7524830823103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>140.9906701536435</v>
+      </c>
+      <c r="E17">
+        <v>-138.5522004143456</v>
+      </c>
+      <c r="F17">
+        <v>2.438469739297844</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1973,12 +2645,18 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>-263.7502309836688</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>0.7860716544951287</v>
+      </c>
+      <c r="E18">
+        <v>-0.6457334086400762</v>
+      </c>
+      <c r="F18">
+        <v>0.1403382458550526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -1987,12 +2665,18 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>-5.298992074751678</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>56.77311781627225</v>
+      </c>
+      <c r="E19">
+        <v>-56.67523976155107</v>
+      </c>
+      <c r="F19">
+        <v>0.09787805472118993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -2001,12 +2685,18 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>-137.9525964481421</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>51.18156226472655</v>
+      </c>
+      <c r="E20">
+        <v>-50.11332675127505</v>
+      </c>
+      <c r="F20">
+        <v>1.06823551345151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -2015,12 +2705,18 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>-282.3247664267045</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>221.7278339474302</v>
+      </c>
+      <c r="E21">
+        <v>-218.9183465233798</v>
+      </c>
+      <c r="F21">
+        <v>2.809487424050428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -2029,12 +2725,18 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <v>23.15551568539471</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>85.23759245409964</v>
+      </c>
+      <c r="E22">
+        <v>-84.30079369195752</v>
+      </c>
+      <c r="F22">
+        <v>0.9367987621421214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2043,12 +2745,18 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>14.43672385837969</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>-43.46649880853853</v>
+      </c>
+      <c r="E23">
+        <v>44.11708992827864</v>
+      </c>
+      <c r="F23">
+        <v>0.6505911197401126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2057,12 +2765,18 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>98.5922422496897</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>-10.09242315308474</v>
+      </c>
+      <c r="E24">
+        <v>10.09490938155504</v>
+      </c>
+      <c r="F24">
+        <v>0.002486228470299778</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B25">
         <v>19</v>
@@ -2071,12 +2785,18 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>-94.20178729717887</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>46.82819967452027</v>
+      </c>
+      <c r="E25">
+        <v>-46.72287908882835</v>
+      </c>
+      <c r="F25">
+        <v>0.1053205856919204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B26">
         <v>20</v>
@@ -2085,12 +2805,18 @@
         <v>23</v>
       </c>
       <c r="D26">
-        <v>-158.2017879371334</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>111.1485009062116</v>
+      </c>
+      <c r="E26">
+        <v>-110.8282003144748</v>
+      </c>
+      <c r="F26">
+        <v>0.320300591736844</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2099,12 +2825,18 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <v>229.1579872779728</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>-65.67029063988511</v>
+      </c>
+      <c r="E27">
+        <v>66.5508225934507</v>
+      </c>
+      <c r="F27">
+        <v>0.8805319535655887</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -2113,12 +2845,18 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>-7.403572784448646</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>-87.55424363225234</v>
+      </c>
+      <c r="E28">
+        <v>87.77117728249596</v>
+      </c>
+      <c r="F28">
+        <v>0.2169336502436225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -2127,12 +2865,18 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>81.95259356654881</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>36.68767643258914</v>
+      </c>
+      <c r="E29">
+        <v>-36.04888030104579</v>
+      </c>
+      <c r="F29">
+        <v>0.638796131543351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B30">
         <v>12</v>
@@ -2141,12 +2885,18 @@
         <v>13</v>
       </c>
       <c r="D30">
-        <v>-385.9392300707591</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>75.72368020563626</v>
+      </c>
+      <c r="E30">
+        <v>-75.35559446873461</v>
+      </c>
+      <c r="F30">
+        <v>0.3680857369016466</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -2155,12 +2905,18 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>158.1579865680637</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>5.38824782838519</v>
+      </c>
+      <c r="E31">
+        <v>-5.329710070023923</v>
+      </c>
+      <c r="F31">
+        <v>0.05853775836126771</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B32">
         <v>19</v>
@@ -2169,12 +2925,18 @@
         <v>20</v>
       </c>
       <c r="D32">
-        <v>-94.20178729717887</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>46.82819967452027</v>
+      </c>
+      <c r="E32">
+        <v>-46.72287908882835</v>
+      </c>
+      <c r="F32">
+        <v>0.1053205856919204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B33">
         <v>15</v>
@@ -2183,12 +2945,18 @@
         <v>21</v>
       </c>
       <c r="D33">
-        <v>-282.3247664267045</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>221.7278339474302</v>
+      </c>
+      <c r="E33">
+        <v>-218.9183465233798</v>
+      </c>
+      <c r="F33">
+        <v>2.809487424050428</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B34">
         <v>18</v>
@@ -2197,7 +2965,13 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>-5.298992074751665</v>
+        <v>56.77311781627225</v>
+      </c>
+      <c r="E34">
+        <v>-56.67523976155107</v>
+      </c>
+      <c r="F34">
+        <v>0.09787805472118993</v>
       </c>
     </row>
   </sheetData>
@@ -2207,29 +2981,35 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>104</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -2238,12 +3018,18 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>53916.26102081346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>110.9326547858927</v>
+      </c>
+      <c r="E2">
+        <v>-110.6323443040448</v>
+      </c>
+      <c r="F2">
+        <v>0.3003104818478874</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -2252,12 +3038,18 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>-53845.69368537825</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>125.6350414727596</v>
+      </c>
+      <c r="E3">
+        <v>-125.2626986355961</v>
+      </c>
+      <c r="F3">
+        <v>0.372342837163453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -2266,12 +3058,18 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>-53128.83517711105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>154.2474499165578</v>
+      </c>
+      <c r="E4">
+        <v>-153.7239816305747</v>
+      </c>
+      <c r="F4">
+        <v>0.523468285983153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2280,12 +3078,18 @@
         <v>24</v>
       </c>
       <c r="D5">
-        <v>-886.8334432983494</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>203.0098915284346</v>
+      </c>
+      <c r="E5">
+        <v>-202.0406029852924</v>
+      </c>
+      <c r="F5">
+        <v>0.9692885431422216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -2294,7 +3098,13 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>53197.10127098116</v>
+        <v>169.227384110226</v>
+      </c>
+      <c r="E6">
+        <v>-168.5895370344083</v>
+      </c>
+      <c r="F6">
+        <v>0.6378470758176658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tap changing transformer model in AC load flow analysis
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -711,7 +711,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>2850.000028498454</v>
+        <v>2850.0000285</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -720,7 +720,7 @@
         <v>2850</v>
       </c>
       <c r="D2">
-        <v>60998.39058607066</v>
+        <v>60998.39019467979</v>
       </c>
     </row>
   </sheetData>
@@ -749,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-1494.485543885834</v>
+        <v>-7.014224642325977</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -757,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1494.577911690925</v>
+        <v>-7.103140916682147</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -765,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-1494.002868075546</v>
+        <v>-6.404042958386182</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -773,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-1497.821079440233</v>
+        <v>-10.23923767718209</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -781,7 +781,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-1497.796678295943</v>
+        <v>-10.39735582046898</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -789,7 +789,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-1500.509804192904</v>
+        <v>-13.14961201638763</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -797,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-1501.147233617722</v>
+        <v>-13.65044939529142</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -805,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-1502.773353373234</v>
+        <v>-15.27657009612768</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -813,7 +813,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-1496.078747561786</v>
+        <v>-8.409271532435426</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -821,7 +821,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-1497.664671451013</v>
+        <v>-10.34058346804791</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -829,7 +829,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-1.913229079300168</v>
+        <v>-2.790266574471174</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -837,7 +837,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-2.896273031906602</v>
+        <v>-2.059230895068654</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -845,7 +845,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1.073799531927371e-21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -853,7 +853,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1.902404339074704</v>
+        <v>1.32057356624658</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -861,7 +861,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10.58924477493816</v>
+        <v>10.28199939289767</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -869,7 +869,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>9.777200096607778</v>
+        <v>9.470095196720891</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -877,7 +877,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>14.53538748605544</v>
+        <v>14.22823343942049</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -885,7 +885,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>16.01842036608769</v>
+        <v>15.71124271994595</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -893,7 +893,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>8.39747018663676</v>
+        <v>8.253737254026634</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -901,7 +901,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>9.268210716243271</v>
+        <v>9.264510898442829</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -909,7 +909,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>16.8549932397513</v>
+        <v>16.54779436894681</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -917,7 +917,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>23.03577256659503</v>
+        <v>22.72859127851293</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -925,7 +925,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>10.53521695993692</v>
+        <v>10.60789884112406</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -933,7 +933,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>4.21269833801922</v>
+        <v>3.904933133453839</v>
       </c>
     </row>
   </sheetData>
@@ -1860,7 +1860,7 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <v>-242.6746623252586</v>
+        <v>-228.8645141549848</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1874,7 +1874,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>53.92242449678692</v>
+        <v>54.9639733419143</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1888,7 +1888,7 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>-179.7486574436127</v>
+        <v>-179.7457971026728</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1902,7 +1902,7 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>-159.1075952696433</v>
+        <v>-159.1080478896982</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1916,7 +1916,7 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>-353.3190588453491</v>
+        <v>-365.6452054346382</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1930,7 +1930,7 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>46.22336118133153</v>
+        <v>46.22338805270467</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1944,7 +1944,7 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>30.4461612684857</v>
+        <v>29.40995031280614</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1958,7 +1958,7 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>-320.6410670758776</v>
+        <v>-320.6377552126719</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1972,7 +1972,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>-29.32442424432037</v>
+        <v>-30.79935817343193</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1986,7 +1986,7 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <v>214.4349330064938</v>
+        <v>214.4524139594521</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2000,7 +2000,7 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <v>-159.3190578943376</v>
+        <v>-171.6452044945984</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2014,7 +2014,7 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>-70.15156886264042</v>
+        <v>-102.309535152862</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2028,7 +2028,7 @@
         <v>23</v>
       </c>
       <c r="D14">
-        <v>-212.5713564885001</v>
+        <v>-214.0378745616294</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2042,7 +2042,7 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>-102.3769934989888</v>
+        <v>-108.5488089415843</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2056,7 +2056,7 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <v>81.92400757320951</v>
+        <v>81.90983487886993</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2070,7 +2070,7 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>-140.892409632265</v>
+        <v>-140.8919581099992</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2084,7 +2084,7 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>-3.988769938099124</v>
+        <v>-5.04246184664594</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2098,7 +2098,7 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>-56.3743284875907</v>
+        <v>-56.3728982163642</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2112,7 +2112,7 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>-70.77099547719999</v>
+        <v>-72.59659034151359</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2126,7 +2126,7 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>-223.1794710464011</v>
+        <v>-223.1811277284571</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2140,7 +2140,7 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <v>-82.07757686312212</v>
+        <v>-81.03602801808567</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2154,7 +2154,7 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>44.67557649558866</v>
+        <v>43.20064256656804</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2168,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>11.59800231417642</v>
+        <v>11.16461687857928</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2182,7 +2182,7 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>-38.37699285903433</v>
+        <v>-44.54880830158424</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2196,7 +2196,7 @@
         <v>23</v>
       </c>
       <c r="D26">
-        <v>-102.3769934989888</v>
+        <v>-108.5488089415842</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2210,7 +2210,7 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <v>68.39076619212186</v>
+        <v>69.87784388796968</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2224,7 +2224,7 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>104.2460160918404</v>
+        <v>91.9023852068315</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2238,7 +2238,7 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>-54.00564505137751</v>
+        <v>-52.18002331578169</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2252,7 +2252,7 @@
         <v>13</v>
       </c>
       <c r="D30">
-        <v>-106.196429502903</v>
+        <v>-75.50495625559178</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2266,7 +2266,7 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>-2.609234517787181</v>
+        <v>-1.122156822030282</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2280,7 +2280,7 @@
         <v>20</v>
       </c>
       <c r="D32">
-        <v>-38.3769928590343</v>
+        <v>-44.54880830158424</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2294,7 +2294,7 @@
         <v>21</v>
       </c>
       <c r="D33">
-        <v>-223.1794710464011</v>
+        <v>-223.1811277284571</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2308,7 +2308,7 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>-56.3743284875907</v>
+        <v>-56.37289821636418</v>
       </c>
     </row>
   </sheetData>
@@ -2349,7 +2349,7 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>-88.6316762178698</v>
+        <v>-116.8893172852906</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2363,7 +2363,7 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>-156.0175839850739</v>
+        <v>-132.0966826668487</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2377,7 +2377,7 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>-140.8389505391082</v>
+        <v>-157.0654223621697</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2391,7 +2391,7 @@
         <v>24</v>
       </c>
       <c r="D5">
-        <v>-214.4349330064938</v>
+        <v>-214.4524139594521</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2405,7 +2405,7 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>-192.8535078430877</v>
+        <v>-172.2727877437279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bugs in the testcase format
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="109">
   <si>
     <t>Conventional generation (MW)</t>
   </si>
@@ -40,181 +40,190 @@
     <t>angle(degs)</t>
   </si>
   <si>
+    <t>Voltage(p.u.)</t>
+  </si>
+  <si>
     <t>busname</t>
   </si>
   <si>
     <t>PD(MW)</t>
   </si>
   <si>
-    <t>alpha</t>
+    <t>QD(MVar)</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D13</t>
   </si>
   <si>
     <t>D14</t>
   </si>
   <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>D18</t>
+  </si>
+  <si>
     <t>D19</t>
   </si>
   <si>
     <t>D2</t>
   </si>
   <si>
+    <t>D20</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
     <t>D8</t>
   </si>
   <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>D16</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>D15</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>D13</t>
-  </si>
-  <si>
-    <t>D20</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D10</t>
-  </si>
-  <si>
     <t>D9</t>
   </si>
   <si>
-    <t>D18</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>PGLB(MW)</t>
+    <t>PG(MW)</t>
   </si>
   <si>
     <t>pG(MW)</t>
   </si>
   <si>
-    <t>PGUB(MW)</t>
+    <t>qG(MVar)</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>G13</t>
+  </si>
+  <si>
+    <t>G14</t>
+  </si>
+  <si>
+    <t>G15</t>
+  </si>
+  <si>
+    <t>G20</t>
+  </si>
+  <si>
+    <t>G17</t>
+  </si>
+  <si>
+    <t>G18</t>
+  </si>
+  <si>
+    <t>G16</t>
+  </si>
+  <si>
+    <t>G21</t>
   </si>
   <si>
     <t>G19</t>
   </si>
   <si>
-    <t>G16</t>
+    <t>G22</t>
+  </si>
+  <si>
+    <t>G23</t>
   </si>
   <si>
     <t>G24</t>
   </si>
   <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G13</t>
-  </si>
-  <si>
-    <t>G10</t>
-  </si>
-  <si>
-    <t>G5</t>
+    <t>G25</t>
+  </si>
+  <si>
+    <t>G29</t>
+  </si>
+  <si>
+    <t>G30</t>
   </si>
   <si>
     <t>G28</t>
   </si>
   <si>
-    <t>G9</t>
-  </si>
-  <si>
-    <t>G17</t>
-  </si>
-  <si>
-    <t>G23</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>G14</t>
-  </si>
-  <si>
-    <t>G11</t>
+    <t>G26</t>
+  </si>
+  <si>
+    <t>G27</t>
+  </si>
+  <si>
+    <t>G32</t>
+  </si>
+  <si>
+    <t>G33</t>
   </si>
   <si>
     <t>G31</t>
   </si>
   <si>
-    <t>G30</t>
-  </si>
-  <si>
-    <t>G25</t>
-  </si>
-  <si>
-    <t>G22</t>
-  </si>
-  <si>
-    <t>G29</t>
-  </si>
-  <si>
-    <t>G7</t>
-  </si>
-  <si>
-    <t>G15</t>
-  </si>
-  <si>
-    <t>G21</t>
-  </si>
-  <si>
-    <t>G8</t>
-  </si>
-  <si>
-    <t>G26</t>
-  </si>
-  <si>
-    <t>G4</t>
-  </si>
-  <si>
-    <t>G18</t>
-  </si>
-  <si>
-    <t>G32</t>
-  </si>
-  <si>
-    <t>G33</t>
-  </si>
-  <si>
-    <t>G6</t>
-  </si>
-  <si>
-    <t>G20</t>
-  </si>
-  <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>G12</t>
-  </si>
-  <si>
-    <t>G27</t>
-  </si>
-  <si>
     <t>from_busname</t>
   </si>
   <si>
     <t>to_busname</t>
   </si>
   <si>
-    <t>pL(MW)</t>
+    <t>pLto(MW)</t>
+  </si>
+  <si>
+    <t>pLfrom(MW)</t>
+  </si>
+  <si>
+    <t>loss(MW)</t>
   </si>
   <si>
     <t>L16-1223</t>
@@ -316,7 +325,13 @@
     <t>L28-1821</t>
   </si>
   <si>
-    <t>pLT(MW)</t>
+    <t>pLTto(MW)</t>
+  </si>
+  <si>
+    <t>pLTfrom(MW)</t>
+  </si>
+  <si>
+    <t>tap</t>
   </si>
   <si>
     <t>T2-911</t>
@@ -711,7 +726,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>2850.0000285</v>
+        <v>2904.200000000004</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -720,7 +735,7 @@
         <v>2850</v>
       </c>
       <c r="D2">
-        <v>60998.39019467979</v>
+        <v>51.70107259315819</v>
       </c>
     </row>
   </sheetData>
@@ -730,210 +745,285 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-7.014224642325977</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>-6.954323538502835</v>
+      </c>
+      <c r="C2">
+        <v>1.04117082822278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-7.103140916682147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>-6.987036112691704</v>
+      </c>
+      <c r="C3">
+        <v>1.035000002455433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-6.404042958386182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>-5.791311160742485</v>
+      </c>
+      <c r="C4">
+        <v>1.049999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-10.23923767718209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>-9.380424379343285</v>
+      </c>
+      <c r="C5">
+        <v>1.006629789036372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-10.39735582046898</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>-9.703130788889492</v>
+      </c>
+      <c r="C6">
+        <v>1.023815596890451</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-13.14961201638763</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>-12.18984802220104</v>
+      </c>
+      <c r="C7">
+        <v>1.015735433141981</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-13.65044939529142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>-7.013805415393748</v>
+      </c>
+      <c r="C8">
+        <v>1.025000002362354</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-15.27657009612768</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>-10.79187799824353</v>
+      </c>
+      <c r="C9">
+        <v>0.9969942998416456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-8.409271532435426</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>-7.255528366266605</v>
+      </c>
+      <c r="C10">
+        <v>1.0167618684634</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-10.34058346804791</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>-9.343244551591434</v>
+      </c>
+      <c r="C11">
+        <v>1.032710786498738</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-2.790266574471174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>-2.175645716463541</v>
+      </c>
+      <c r="C12">
+        <v>0.9934632329817151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-2.059230895068654</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>-1.519621563376003</v>
+      </c>
+      <c r="C13">
+        <v>1.007024401032142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>4.221759495687971e-20</v>
+      </c>
+      <c r="C14">
+        <v>1.020000001888093</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1.32057356624658</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>2.116495859886609</v>
+      </c>
+      <c r="C15">
+        <v>0.9800000080843081</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10.28199939289767</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>10.47761278022463</v>
+      </c>
+      <c r="C16">
+        <v>1.095787515001609</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>9.470095196720891</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>9.901489759718437</v>
+      </c>
+      <c r="C17">
+        <v>1.035523049175849</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>14.22823343942049</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>14.21566969594195</v>
+      </c>
+      <c r="C18">
+        <v>1.044723693697603</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>15.71124271994595</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>15.536375327696</v>
+      </c>
+      <c r="C19">
+        <v>1.049999999486777</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>8.253737254026634</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>8.557751830377441</v>
+      </c>
+      <c r="C20">
+        <v>1.033921930874467</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>9.264510898442829</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>9.284541202331065</v>
+      </c>
+      <c r="C21">
+        <v>1.042247776687631</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>16.54779436894681</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>16.29524219487851</v>
+      </c>
+      <c r="C22">
+        <v>1.050001127725279</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>22.72859127851293</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>21.98421337364544</v>
+      </c>
+      <c r="C23">
+        <v>1.050000000301776</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>10.60789884112406</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>10.38975429877364</v>
+      </c>
+      <c r="C24">
+        <v>1.0500000010586</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>3.904933133453839</v>
+        <v>4.964785223388745</v>
+      </c>
+      <c r="C25">
+        <v>1.027050699266258</v>
       </c>
     </row>
   </sheetData>
@@ -954,88 +1044,88 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>194</v>
+        <v>108</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>19</v>
-      </c>
       <c r="C3">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>97</v>
+        <v>265</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>71</v>
+        <v>317</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -1044,161 +1134,161 @@
         <v>100</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>125</v>
+        <v>333</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>317</v>
+        <v>181</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>265</v>
+        <v>128</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>128</v>
+        <v>180</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>180</v>
+        <v>71</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>195</v>
+        <v>136</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>333</v>
+        <v>171</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>108</v>
+        <v>175</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1219,67 +1309,67 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2">
-        <v>2.4</v>
+        <v>76</v>
       </c>
       <c r="D2">
-        <v>2.4</v>
+        <v>76</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>10.467</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3">
-        <v>2.4</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>2.4</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>10.467</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>400</v>
+        <v>10.467</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1287,50 +1377,50 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>10.467</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="D6">
-        <v>76.259</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>197</v>
+        <v>-9.763</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="D7">
-        <v>57.074</v>
+        <v>76</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>-9.763</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1338,33 +1428,33 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>20</v>
+        <v>-9.763</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="E9">
-        <v>50</v>
+        <v>-9.763</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1372,67 +1462,67 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="D10">
-        <v>57.074</v>
+        <v>80</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>14.906</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11">
-        <v>2.4</v>
+        <v>80</v>
       </c>
       <c r="D11">
-        <v>2.4</v>
+        <v>80</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>14.906</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D12">
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="E12">
-        <v>400</v>
+        <v>14.906</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13">
-        <v>15.2</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="D13">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>76</v>
+        <v>38.554</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1440,356 +1530,356 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14">
-        <v>69</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="D14">
-        <v>76.259</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="E14">
-        <v>197</v>
+        <v>38.554</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15">
-        <v>25</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="D15">
-        <v>57.074</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="E15">
-        <v>100</v>
+        <v>38.554</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16">
-        <v>54.3</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>155</v>
+        <v>-85.18899999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D17">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E17">
-        <v>50</v>
+        <v>137.038</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D18">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E18">
-        <v>50</v>
+        <v>137.038</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19">
-        <v>54.3</v>
+        <v>12</v>
       </c>
       <c r="D19">
-        <v>155</v>
+        <v>12</v>
       </c>
       <c r="E19">
-        <v>155</v>
+        <v>137.038</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D20">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E20">
-        <v>50</v>
+        <v>137.038</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21">
-        <v>15.2</v>
+        <v>155</v>
       </c>
       <c r="D21">
-        <v>76</v>
+        <v>155</v>
       </c>
       <c r="E21">
-        <v>76</v>
+        <v>137.038</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>137.038</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23">
-        <v>54.3</v>
+        <v>155</v>
       </c>
       <c r="D23">
         <v>155</v>
       </c>
       <c r="E23">
-        <v>155</v>
+        <v>-204.617</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24">
-        <v>15.2</v>
+        <v>400</v>
       </c>
       <c r="D24">
-        <v>76</v>
+        <v>400</v>
       </c>
       <c r="E24">
-        <v>76</v>
+        <v>93.44799999999999</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25">
-        <v>10</v>
+        <v>400</v>
       </c>
       <c r="D25">
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="E25">
-        <v>50</v>
+        <v>-239.827</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26">
-        <v>15.2</v>
+        <v>50</v>
       </c>
       <c r="D26">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="E26">
-        <v>76</v>
+        <v>-5.949</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27">
-        <v>2.4</v>
+        <v>50</v>
       </c>
       <c r="D27">
-        <v>2.4</v>
+        <v>50</v>
       </c>
       <c r="E27">
-        <v>12</v>
+        <v>-5.949</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28">
-        <v>54.3</v>
+        <v>50</v>
       </c>
       <c r="D28">
-        <v>155</v>
+        <v>50</v>
       </c>
       <c r="E28">
-        <v>155</v>
+        <v>-5.949</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C29">
-        <v>140</v>
+        <v>50</v>
       </c>
       <c r="D29">
-        <v>350</v>
+        <v>50</v>
       </c>
       <c r="E29">
-        <v>350</v>
+        <v>-5.949</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C30">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D30">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>-5.949</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31">
-        <v>2.4</v>
+        <v>50</v>
       </c>
       <c r="D31">
-        <v>2.4</v>
+        <v>50</v>
       </c>
       <c r="E31">
-        <v>12</v>
+        <v>-5.949</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C32">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="D32">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="E32">
-        <v>20</v>
+        <v>31.016</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C33">
-        <v>69</v>
+        <v>350</v>
       </c>
       <c r="D33">
-        <v>76.259</v>
+        <v>350</v>
       </c>
       <c r="E33">
-        <v>197</v>
+        <v>31.016</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="D34">
-        <v>50</v>
+        <v>155</v>
       </c>
       <c r="E34">
-        <v>50</v>
+        <v>31.016</v>
       </c>
     </row>
   </sheetData>
@@ -1810,16 +1900,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1829,29 +1919,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>65</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1860,12 +1956,18 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <v>-228.8645141549848</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>231.0973846062458</v>
+      </c>
+      <c r="E2">
+        <v>-224.9052493739453</v>
+      </c>
+      <c r="F2">
+        <v>6.192135232300444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1874,12 +1976,18 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>54.9639733419143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>-48.45929200953859</v>
+      </c>
+      <c r="E3">
+        <v>49.60074781399344</v>
+      </c>
+      <c r="F3">
+        <v>1.141455804454855</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -1888,12 +1996,18 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>-179.7457971026728</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>177.8622472010045</v>
+      </c>
+      <c r="E4">
+        <v>-177.3403116581501</v>
+      </c>
+      <c r="F4">
+        <v>0.5219355428544903</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -1902,12 +2016,18 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>-159.1080478896982</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>159.592863284746</v>
+      </c>
+      <c r="E5">
+        <v>-157.5707215604764</v>
+      </c>
+      <c r="F5">
+        <v>2.022141724269666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -1916,12 +2036,18 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>-365.6452054346382</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>369.3602085196973</v>
+      </c>
+      <c r="E6">
+        <v>-362.2775765304243</v>
+      </c>
+      <c r="F6">
+        <v>7.08263198927308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1930,12 +2056,18 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>46.22338805270467</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>-112.9343942867115</v>
+      </c>
+      <c r="E7">
+        <v>115.0000000000011</v>
+      </c>
+      <c r="F7">
+        <v>2.065605713289664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1944,12 +2076,18 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>29.40995031280614</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>-28.30296306950447</v>
+      </c>
+      <c r="E8">
+        <v>28.67028120670147</v>
+      </c>
+      <c r="F8">
+        <v>0.3673181371970036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -1958,12 +2096,18 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>-320.6377552126719</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>315.3322318685674</v>
+      </c>
+      <c r="E9">
+        <v>-312.323499216732</v>
+      </c>
+      <c r="F9">
+        <v>3.008732651835411</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1972,12 +2116,18 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>-30.79935817343193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>36.87524112000978</v>
+      </c>
+      <c r="E10">
+        <v>-36.52243142367535</v>
+      </c>
+      <c r="F10">
+        <v>0.3528096963344218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B11">
         <v>15</v>
@@ -1986,12 +2136,18 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <v>214.4524139594521</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>-220.9043010387272</v>
+      </c>
+      <c r="E11">
+        <v>224.6073721434057</v>
+      </c>
+      <c r="F11">
+        <v>3.703071104678513</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -2000,12 +2156,18 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <v>-171.6452044945984</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>168.2775755304249</v>
+      </c>
+      <c r="E12">
+        <v>-166.5623896137328</v>
+      </c>
+      <c r="F12">
+        <v>1.715185916692152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -2014,12 +2176,18 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>-102.309535152862</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>86.87483976711863</v>
+      </c>
+      <c r="E13">
+        <v>-86.30134885151266</v>
+      </c>
+      <c r="F13">
+        <v>0.5734909156059675</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2028,12 +2196,18 @@
         <v>23</v>
       </c>
       <c r="D14">
-        <v>-214.0378745616294</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>226.8349381744235</v>
+      </c>
+      <c r="E14">
+        <v>-221.5777826725933</v>
+      </c>
+      <c r="F14">
+        <v>5.257155501830235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -2042,12 +2216,18 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>-108.5488089415843</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>101.0338386096659</v>
+      </c>
+      <c r="E15">
+        <v>-100.7580387932958</v>
+      </c>
+      <c r="F15">
+        <v>0.2757998163700481</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -2056,12 +2236,18 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <v>81.90983487886993</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>-110.0029129863685</v>
+      </c>
+      <c r="E16">
+        <v>112.7130610828596</v>
+      </c>
+      <c r="F16">
+        <v>2.710148096491172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -2070,12 +2256,18 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>-140.8919581099992</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>140.4071367152556</v>
+      </c>
+      <c r="E17">
+        <v>-137.991920210417</v>
+      </c>
+      <c r="F17">
+        <v>2.415216504838624</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2084,12 +2276,18 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>-5.04246184664594</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>10.93763466232599</v>
+      </c>
+      <c r="E18">
+        <v>-10.87700970800601</v>
+      </c>
+      <c r="F18">
+        <v>0.06062495431997938</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -2098,12 +2296,18 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>-56.3728982163642</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>55.52474588094621</v>
+      </c>
+      <c r="E19">
+        <v>-55.43112360050198</v>
+      </c>
+      <c r="F19">
+        <v>0.09362228044423881</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -2112,12 +2316,18 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>-72.59659034151359</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>38.73237685987056</v>
+      </c>
+      <c r="E20">
+        <v>-38.10817160533062</v>
+      </c>
+      <c r="F20">
+        <v>0.624205254539939</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -2126,12 +2336,18 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>-223.1811277284571</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>223.2606148992922</v>
+      </c>
+      <c r="E21">
+        <v>-219.6602166131318</v>
+      </c>
+      <c r="F21">
+        <v>3.600398286160456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -2140,12 +2356,18 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <v>-81.03602801808567</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>88.5784283000702</v>
+      </c>
+      <c r="E22">
+        <v>-87.54070799046096</v>
+      </c>
+      <c r="F22">
+        <v>1.037720309609247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2154,12 +2376,18 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>43.20064256656804</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>-37.47756857632417</v>
+      </c>
+      <c r="E23">
+        <v>37.97977196480572</v>
+      </c>
+      <c r="F23">
+        <v>0.5022033884815424</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2168,12 +2396,18 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>11.16461687857928</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>-12.58051977879781</v>
+      </c>
+      <c r="E24">
+        <v>12.63048672482128</v>
+      </c>
+      <c r="F24">
+        <v>0.04996694602347196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B25">
         <v>19</v>
@@ -2182,12 +2416,18 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>-44.54880830158424</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>36.75803879329603</v>
+      </c>
+      <c r="E25">
+        <v>-36.68039205606517</v>
+      </c>
+      <c r="F25">
+        <v>0.07764673723086313</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B26">
         <v>20</v>
@@ -2196,12 +2436,18 @@
         <v>23</v>
       </c>
       <c r="D26">
-        <v>-108.5488089415842</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>101.0338386096659</v>
+      </c>
+      <c r="E26">
+        <v>-100.7580387932958</v>
+      </c>
+      <c r="F26">
+        <v>0.2757998163700481</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2210,12 +2456,18 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <v>69.87784388796968</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>-61.4580981947222</v>
+      </c>
+      <c r="E27">
+        <v>62.2465229831861</v>
+      </c>
+      <c r="F27">
+        <v>0.788424788463904</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -2224,12 +2476,18 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>91.9023852068315</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>-107.6392158878692</v>
+      </c>
+      <c r="E28">
+        <v>107.9662036834029</v>
+      </c>
+      <c r="F28">
+        <v>0.326987795533662</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -2238,12 +2496,18 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>-52.18002331578169</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>20.24137494942709</v>
+      </c>
+      <c r="E29">
+        <v>-19.95743410795746</v>
+      </c>
+      <c r="F29">
+        <v>0.2839408414696321</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B30">
         <v>12</v>
@@ -2252,12 +2516,18 @@
         <v>13</v>
       </c>
       <c r="D30">
-        <v>-75.50495625559178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>59.90294190801899</v>
+      </c>
+      <c r="E30">
+        <v>-59.66697230505906</v>
+      </c>
+      <c r="F30">
+        <v>0.235969602959929</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -2266,12 +2536,18 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>-1.122156822030282</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>9.575029256403427</v>
+      </c>
+      <c r="E31">
+        <v>-9.541901805277332</v>
+      </c>
+      <c r="F31">
+        <v>0.03312745112609566</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B32">
         <v>19</v>
@@ -2280,12 +2556,18 @@
         <v>20</v>
       </c>
       <c r="D32">
-        <v>-44.54880830158424</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>36.75803879329603</v>
+      </c>
+      <c r="E32">
+        <v>-36.68039205606517</v>
+      </c>
+      <c r="F32">
+        <v>0.07764673723086313</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B33">
         <v>15</v>
@@ -2294,12 +2576,18 @@
         <v>21</v>
       </c>
       <c r="D33">
-        <v>-223.1811277284571</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>223.2606148992922</v>
+      </c>
+      <c r="E33">
+        <v>-219.6602166131318</v>
+      </c>
+      <c r="F33">
+        <v>3.600398286160456</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B34">
         <v>18</v>
@@ -2308,7 +2596,13 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>-56.37289821636418</v>
+        <v>55.52474588094621</v>
+      </c>
+      <c r="E34">
+        <v>-55.43112360050198</v>
+      </c>
+      <c r="F34">
+        <v>0.09362228044423881</v>
       </c>
     </row>
   </sheetData>
@@ -2318,29 +2612,38 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>101</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -2349,12 +2652,21 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>-116.8893172852906</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>103.7513389609836</v>
+      </c>
+      <c r="E2">
+        <v>-103.498507010708</v>
+      </c>
+      <c r="F2">
+        <v>0.2528319502756116</v>
+      </c>
+      <c r="G2">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -2363,12 +2675,21 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>-132.0966826668487</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>119.1440568789012</v>
+      </c>
+      <c r="E3">
+        <v>-118.8061478996674</v>
+      </c>
+      <c r="F3">
+        <v>0.3379089792338252</v>
+      </c>
+      <c r="G3">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -2377,12 +2698,21 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>-157.0654223621697</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>149.1123995042622</v>
+      </c>
+      <c r="E4">
+        <v>-148.5873477006254</v>
+      </c>
+      <c r="F4">
+        <v>0.525051803636889</v>
+      </c>
+      <c r="G4">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2391,12 +2721,21 @@
         <v>24</v>
       </c>
       <c r="D5">
-        <v>-214.4524139594521</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>220.9043010387276</v>
+      </c>
+      <c r="E5">
+        <v>-219.607915869027</v>
+      </c>
+      <c r="F5">
+        <v>1.296385169700631</v>
+      </c>
+      <c r="G5">
+        <v>1.100000010651292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -2405,7 +2744,16 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>-172.2727877437279</v>
+        <v>165.4281648001037</v>
+      </c>
+      <c r="E6">
+        <v>-164.8074848052748</v>
+      </c>
+      <c r="F6">
+        <v>0.6206799948288211</v>
+      </c>
+      <c r="G6">
+        <v>1.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data printing issues resolved
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -726,7 +726,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>2904.200000000004</v>
+        <v>2904.199958328551</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -735,7 +735,7 @@
         <v>2850</v>
       </c>
       <c r="D2">
-        <v>51.70107259315819</v>
+        <v>51.70103124997319</v>
       </c>
     </row>
   </sheetData>
@@ -767,10 +767,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-6.954323538502835</v>
+        <v>-6.954336164209468</v>
       </c>
       <c r="C2">
-        <v>1.04117082822278</v>
+        <v>1.041171740726286</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -778,10 +778,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-6.987036112691704</v>
+        <v>-6.987038895179992</v>
       </c>
       <c r="C3">
-        <v>1.035000002455433</v>
+        <v>1.035000000900278</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -789,10 +789,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-5.791311160742485</v>
+        <v>-5.791314030672015</v>
       </c>
       <c r="C4">
-        <v>1.049999999999991</v>
+        <v>1.049999989553545</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -800,10 +800,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-9.380424379343285</v>
+        <v>-9.380426072626054</v>
       </c>
       <c r="C5">
-        <v>1.006629789036372</v>
+        <v>1.006629803587966</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -811,10 +811,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-9.703130788889492</v>
+        <v>-9.703135100475894</v>
       </c>
       <c r="C6">
-        <v>1.023815596890451</v>
+        <v>1.023816162635372</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -822,10 +822,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-12.18984802220104</v>
+        <v>-12.18984785700471</v>
       </c>
       <c r="C7">
-        <v>1.015735433141981</v>
+        <v>1.015735577424695</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -833,10 +833,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-7.013805415393748</v>
+        <v>-7.0138043603139</v>
       </c>
       <c r="C8">
-        <v>1.025000002362354</v>
+        <v>1.025000000861727</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -844,10 +844,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-10.79187799824353</v>
+        <v>-10.7918773526312</v>
       </c>
       <c r="C9">
-        <v>0.9969942998416456</v>
+        <v>0.996994344779235</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -855,10 +855,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-7.255528366266605</v>
+        <v>-7.255529263787974</v>
       </c>
       <c r="C10">
-        <v>1.0167618684634</v>
+        <v>1.016761895503189</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -866,10 +866,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-9.343244551591434</v>
+        <v>-9.343244474360933</v>
       </c>
       <c r="C11">
-        <v>1.032710786498738</v>
+        <v>1.032710967342917</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -877,10 +877,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-2.175645716463541</v>
+        <v>-2.175645845717776</v>
       </c>
       <c r="C12">
-        <v>0.9934632329817151</v>
+        <v>0.993463264623684</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -888,10 +888,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-1.519621563376003</v>
+        <v>-1.519622106706469</v>
       </c>
       <c r="C13">
-        <v>1.007024401032142</v>
+        <v>1.007024443039843</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -899,10 +899,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4.221759495687971e-20</v>
+        <v>1.922255097482938e-22</v>
       </c>
       <c r="C14">
-        <v>1.020000001888093</v>
+        <v>1.020000000687559</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -910,10 +910,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2.116495859886609</v>
+        <v>2.116497042707441</v>
       </c>
       <c r="C15">
-        <v>0.9800000080843081</v>
+        <v>0.9800000029333509</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -921,10 +921,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10.47761278022463</v>
+        <v>10.47761840216531</v>
       </c>
       <c r="C16">
-        <v>1.095787515001609</v>
+        <v>1.09578684298166</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -932,10 +932,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>9.901489759718437</v>
+        <v>9.901490906490791</v>
       </c>
       <c r="C17">
-        <v>1.035523049175849</v>
+        <v>1.03552312332949</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -943,10 +943,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>14.21566969594195</v>
+        <v>14.21567334744549</v>
       </c>
       <c r="C18">
-        <v>1.044723693697603</v>
+        <v>1.044723716059756</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -954,10 +954,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>15.536375327696</v>
+        <v>15.53637998996704</v>
       </c>
       <c r="C19">
-        <v>1.049999999486777</v>
+        <v>1.049999999808577</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -965,10 +965,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>8.557751830377441</v>
+        <v>8.557752832219609</v>
       </c>
       <c r="C20">
-        <v>1.033921930874467</v>
+        <v>1.033921973285685</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -976,10 +976,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>9.284541202331065</v>
+        <v>9.284541911580224</v>
       </c>
       <c r="C21">
-        <v>1.042247776687631</v>
+        <v>1.042247791338515</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -987,10 +987,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>16.29524219487851</v>
+        <v>16.29525361727388</v>
       </c>
       <c r="C22">
-        <v>1.050001127725279</v>
+        <v>1.050000356255982</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -998,10 +998,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>21.98421337364544</v>
+        <v>21.98422090266471</v>
       </c>
       <c r="C23">
-        <v>1.050000000301776</v>
+        <v>1.050000000112305</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1009,10 +1009,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>10.38975429877364</v>
+        <v>10.38975485847643</v>
       </c>
       <c r="C24">
-        <v>1.0500000010586</v>
+        <v>1.050000000393651</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1020,10 +1020,10 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>4.964785223388745</v>
+        <v>4.964784838117613</v>
       </c>
       <c r="C25">
-        <v>1.027050699266258</v>
+        <v>1.027050270768929</v>
       </c>
     </row>
   </sheetData>
@@ -1335,7 +1335,7 @@
         <v>76</v>
       </c>
       <c r="E2">
-        <v>10.467</v>
+        <v>10.469</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1352,7 +1352,7 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>10.467</v>
+        <v>10.469</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1369,7 +1369,7 @@
         <v>10</v>
       </c>
       <c r="E4">
-        <v>10.467</v>
+        <v>10.469</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1386,7 +1386,7 @@
         <v>76</v>
       </c>
       <c r="E5">
-        <v>10.467</v>
+        <v>10.469</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1403,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>-9.763</v>
+        <v>-9.765000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1420,7 +1420,7 @@
         <v>76</v>
       </c>
       <c r="E7">
-        <v>-9.763</v>
+        <v>-9.765000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1437,7 +1437,7 @@
         <v>10</v>
       </c>
       <c r="E8">
-        <v>-9.763</v>
+        <v>-9.765000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1454,7 +1454,7 @@
         <v>76</v>
       </c>
       <c r="E9">
-        <v>-9.763</v>
+        <v>-9.765000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1590,7 +1590,7 @@
         <v>12</v>
       </c>
       <c r="E17">
-        <v>137.038</v>
+        <v>137.037</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1607,7 +1607,7 @@
         <v>12</v>
       </c>
       <c r="E18">
-        <v>137.038</v>
+        <v>137.037</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1624,7 +1624,7 @@
         <v>12</v>
       </c>
       <c r="E19">
-        <v>137.038</v>
+        <v>137.037</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1641,7 +1641,7 @@
         <v>12</v>
       </c>
       <c r="E20">
-        <v>137.038</v>
+        <v>137.037</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1658,7 +1658,7 @@
         <v>155</v>
       </c>
       <c r="E21">
-        <v>137.038</v>
+        <v>137.037</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1675,7 +1675,7 @@
         <v>12</v>
       </c>
       <c r="E22">
-        <v>137.038</v>
+        <v>137.037</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1692,7 +1692,7 @@
         <v>155</v>
       </c>
       <c r="E23">
-        <v>-204.617</v>
+        <v>-204.612</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1709,7 +1709,7 @@
         <v>400</v>
       </c>
       <c r="E24">
-        <v>93.44799999999999</v>
+        <v>93.45399999999999</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1726,7 +1726,7 @@
         <v>400</v>
       </c>
       <c r="E25">
-        <v>-239.827</v>
+        <v>-239.835</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1956,13 +1956,13 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <v>231.0973846062458</v>
+        <v>231.0974088300875</v>
       </c>
       <c r="E2">
-        <v>-224.9052493739453</v>
+        <v>-224.9052727344524</v>
       </c>
       <c r="F2">
-        <v>6.192135232300444</v>
+        <v>6.192136095635004</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1976,13 +1976,13 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>-48.45929200953859</v>
+        <v>-48.45925443476258</v>
       </c>
       <c r="E3">
-        <v>49.60074781399344</v>
+        <v>49.60070844371397</v>
       </c>
       <c r="F3">
-        <v>1.141455804454855</v>
+        <v>1.141454008951392</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1996,13 +1996,13 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>177.8622472010045</v>
+        <v>177.8623638468168</v>
       </c>
       <c r="E4">
-        <v>-177.3403116581501</v>
+        <v>-177.3404277294767</v>
       </c>
       <c r="F4">
-        <v>0.5219355428544903</v>
+        <v>0.5219361173400383</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2016,13 +2016,13 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>159.592863284746</v>
+        <v>159.5927872348254</v>
       </c>
       <c r="E5">
-        <v>-157.5707215604764</v>
+        <v>-157.5706497575499</v>
       </c>
       <c r="F5">
-        <v>2.022141724269666</v>
+        <v>2.022137477275576</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2036,13 +2036,13 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>369.3602085196973</v>
+        <v>369.3602581928429</v>
       </c>
       <c r="E6">
-        <v>-362.2775765304243</v>
+        <v>-362.277622993714</v>
       </c>
       <c r="F6">
-        <v>7.08263198927308</v>
+        <v>7.082635199128884</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2056,13 +2056,13 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>-112.9343942867115</v>
+        <v>-112.9343918605495</v>
       </c>
       <c r="E7">
-        <v>115.0000000000011</v>
+        <v>114.9999970027528</v>
       </c>
       <c r="F7">
-        <v>2.065605713289664</v>
+        <v>2.065605142203308</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2076,13 +2076,13 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>-28.30296306950447</v>
+        <v>-28.30292709544883</v>
       </c>
       <c r="E8">
-        <v>28.67028120670147</v>
+        <v>28.67024434418971</v>
       </c>
       <c r="F8">
-        <v>0.3673181371970036</v>
+        <v>0.3673172487408782</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2096,13 +2096,13 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>315.3322318685674</v>
+        <v>315.3324155686497</v>
       </c>
       <c r="E9">
-        <v>-312.323499216732</v>
+        <v>-312.323679657658</v>
       </c>
       <c r="F9">
-        <v>3.008732651835411</v>
+        <v>3.008735910991645</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2116,13 +2116,13 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>36.87524112000978</v>
+        <v>36.87525852921386</v>
       </c>
       <c r="E10">
-        <v>-36.52243142367535</v>
+        <v>-36.52244851399961</v>
       </c>
       <c r="F10">
-        <v>0.3528096963344218</v>
+        <v>0.3528100152142499</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2136,13 +2136,13 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <v>-220.9043010387272</v>
+        <v>-220.9042426163613</v>
       </c>
       <c r="E11">
-        <v>224.6073721434057</v>
+        <v>224.6073084525962</v>
       </c>
       <c r="F11">
-        <v>3.703071104678513</v>
+        <v>3.703065836234876</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2156,13 +2156,13 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <v>168.2775755304249</v>
+        <v>168.2776219955612</v>
       </c>
       <c r="E12">
-        <v>-166.5623896137328</v>
+        <v>-166.5624347190722</v>
       </c>
       <c r="F12">
-        <v>1.715185916692152</v>
+        <v>1.715187276489027</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2176,13 +2176,13 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>86.87483976711863</v>
+        <v>86.87483807478857</v>
       </c>
       <c r="E13">
-        <v>-86.30134885151266</v>
+        <v>-86.30134756302856</v>
       </c>
       <c r="F13">
-        <v>0.5734909156059675</v>
+        <v>0.5734905117600109</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2196,13 +2196,13 @@
         <v>23</v>
       </c>
       <c r="D14">
-        <v>226.8349381744235</v>
+        <v>226.8349498303853</v>
       </c>
       <c r="E14">
-        <v>-221.5777826725933</v>
+        <v>-221.5777937823791</v>
       </c>
       <c r="F14">
-        <v>5.257155501830235</v>
+        <v>5.257156048006184</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2216,13 +2216,13 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>101.0338386096659</v>
+        <v>101.0338173711477</v>
       </c>
       <c r="E15">
-        <v>-100.7580387932958</v>
+        <v>-100.7580177567392</v>
       </c>
       <c r="F15">
-        <v>0.2757998163700481</v>
+        <v>0.2757996144084673</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2236,13 +2236,13 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <v>-110.0029129863685</v>
+        <v>-110.0028256249187</v>
       </c>
       <c r="E16">
-        <v>112.7130610828596</v>
+        <v>112.7129099135157</v>
       </c>
       <c r="F16">
-        <v>2.710148096491172</v>
+        <v>2.710084288597092</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2256,13 +2256,13 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>140.4071367152556</v>
+        <v>140.4072067707107</v>
       </c>
       <c r="E17">
-        <v>-137.991920210417</v>
+        <v>-137.991987839173</v>
       </c>
       <c r="F17">
-        <v>2.415216504838624</v>
+        <v>2.41521893153771</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2276,13 +2276,13 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>10.93763466232599</v>
+        <v>10.93761504779571</v>
       </c>
       <c r="E18">
-        <v>-10.87700970800601</v>
+        <v>-10.87699104974649</v>
       </c>
       <c r="F18">
-        <v>0.06062495431997938</v>
+        <v>0.06062399804922375</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2296,13 +2296,13 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>55.52474588094621</v>
+        <v>55.52480781459366</v>
       </c>
       <c r="E19">
-        <v>-55.43112360050198</v>
+        <v>-55.43118392294721</v>
       </c>
       <c r="F19">
-        <v>0.09362228044423881</v>
+        <v>0.0936238916464438</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2316,13 +2316,13 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>38.73237685987056</v>
+        <v>38.732361113112</v>
       </c>
       <c r="E20">
-        <v>-38.10817160533062</v>
+        <v>-38.10815641637365</v>
       </c>
       <c r="F20">
-        <v>0.624205254539939</v>
+        <v>0.6242046967383508</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2336,13 +2336,13 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>223.2606148992922</v>
+        <v>223.2605150646424</v>
       </c>
       <c r="E21">
-        <v>-219.6602166131318</v>
+        <v>-219.6601124552858</v>
       </c>
       <c r="F21">
-        <v>3.600398286160456</v>
+        <v>3.600402609356612</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2356,13 +2356,13 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <v>88.5784283000702</v>
+        <v>88.57846656106835</v>
       </c>
       <c r="E22">
-        <v>-87.54070799046096</v>
+        <v>-87.54074556523743</v>
       </c>
       <c r="F22">
-        <v>1.037720309609247</v>
+        <v>1.037720995830915</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2376,13 +2376,13 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>-37.47756857632417</v>
+        <v>-37.47755148600039</v>
       </c>
       <c r="E23">
-        <v>37.97977196480572</v>
+        <v>37.97975438722105</v>
       </c>
       <c r="F23">
-        <v>0.5022033884815424</v>
+        <v>0.5022029012206608</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2396,13 +2396,13 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>-12.58051977879781</v>
+        <v>-12.58046682726585</v>
       </c>
       <c r="E24">
-        <v>12.63048672482128</v>
+        <v>12.63044818795772</v>
       </c>
       <c r="F24">
-        <v>0.04996694602347196</v>
+        <v>0.04998136069186976</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2416,13 +2416,13 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>36.75803879329603</v>
+        <v>36.75801775673923</v>
       </c>
       <c r="E25">
-        <v>-36.68039205606517</v>
+        <v>-36.68037120899265</v>
       </c>
       <c r="F25">
-        <v>0.07764673723086313</v>
+        <v>0.07764654774657376</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2436,13 +2436,13 @@
         <v>23</v>
       </c>
       <c r="D26">
-        <v>101.0338386096659</v>
+        <v>101.0338173711477</v>
       </c>
       <c r="E26">
-        <v>-100.7580387932958</v>
+        <v>-100.7580177567392</v>
       </c>
       <c r="F26">
-        <v>0.2757998163700481</v>
+        <v>0.2757996144084673</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2456,13 +2456,13 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <v>-61.4580981947222</v>
+        <v>-61.45811387440724</v>
       </c>
       <c r="E27">
-        <v>62.2465229831861</v>
+        <v>62.24653886545782</v>
       </c>
       <c r="F27">
-        <v>0.788424788463904</v>
+        <v>0.7884249910505847</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2476,13 +2476,13 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>-107.6392158878692</v>
+        <v>-107.6392575820147</v>
       </c>
       <c r="E28">
-        <v>107.9662036834029</v>
+        <v>107.9662455406568</v>
       </c>
       <c r="F28">
-        <v>0.326987795533662</v>
+        <v>0.326987958642122</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2496,13 +2496,13 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>20.24137494942709</v>
+        <v>20.2413939355046</v>
       </c>
       <c r="E29">
-        <v>-19.95743410795746</v>
+        <v>-19.95745172307686</v>
       </c>
       <c r="F29">
-        <v>0.2839408414696321</v>
+        <v>0.283942212427743</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2516,13 +2516,13 @@
         <v>13</v>
       </c>
       <c r="D30">
-        <v>59.90294190801899</v>
+        <v>59.90295271036039</v>
       </c>
       <c r="E30">
-        <v>-59.66697230505906</v>
+        <v>-59.66698325979712</v>
       </c>
       <c r="F30">
-        <v>0.235969602959929</v>
+        <v>0.235969450563267</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2536,13 +2536,13 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>9.575029256403427</v>
+        <v>9.575011987546883</v>
       </c>
       <c r="E31">
-        <v>-9.541901805277332</v>
+        <v>-9.541886125592757</v>
       </c>
       <c r="F31">
-        <v>0.03312745112609566</v>
+        <v>0.03312586195412526</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2556,13 +2556,13 @@
         <v>20</v>
       </c>
       <c r="D32">
-        <v>36.75803879329603</v>
+        <v>36.75801775673923</v>
       </c>
       <c r="E32">
-        <v>-36.68039205606517</v>
+        <v>-36.68037120899265</v>
       </c>
       <c r="F32">
-        <v>0.07764673723086313</v>
+        <v>0.07764654774657376</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2576,13 +2576,13 @@
         <v>21</v>
       </c>
       <c r="D33">
-        <v>223.2606148992922</v>
+        <v>223.2605150646424</v>
       </c>
       <c r="E33">
-        <v>-219.6602166131318</v>
+        <v>-219.6601124552858</v>
       </c>
       <c r="F33">
-        <v>3.600398286160456</v>
+        <v>3.600402609356612</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2596,13 +2596,13 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>55.52474588094621</v>
+        <v>55.52480781459366</v>
       </c>
       <c r="E34">
-        <v>-55.43112360050198</v>
+        <v>-55.43118392294721</v>
       </c>
       <c r="F34">
-        <v>0.09362228044423881</v>
+        <v>0.0936238916464438</v>
       </c>
     </row>
   </sheetData>
@@ -2652,13 +2652,13 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>103.7513389609836</v>
+        <v>103.751360831875</v>
       </c>
       <c r="E2">
-        <v>-103.498507010708</v>
+        <v>-103.498528788644</v>
       </c>
       <c r="F2">
-        <v>0.2528319502756116</v>
+        <v>0.2528320432310105</v>
       </c>
       <c r="G2">
         <v>1.03</v>
@@ -2675,13 +2675,13 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>119.1440568789012</v>
+        <v>119.1440728202233</v>
       </c>
       <c r="E3">
-        <v>-118.8061478996674</v>
+        <v>-118.8061637582331</v>
       </c>
       <c r="F3">
-        <v>0.3379089792338252</v>
+        <v>0.3379090619902048</v>
       </c>
       <c r="G3">
         <v>1.03</v>
@@ -2698,13 +2698,13 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>149.1123995042622</v>
+        <v>149.1124214502258</v>
       </c>
       <c r="E4">
-        <v>-148.5873477006254</v>
+        <v>-148.5873693891832</v>
       </c>
       <c r="F4">
-        <v>0.525051803636889</v>
+        <v>0.5250520610425191</v>
       </c>
       <c r="G4">
         <v>1.02</v>
@@ -2721,16 +2721,16 @@
         <v>24</v>
       </c>
       <c r="D5">
-        <v>220.9043010387276</v>
+        <v>220.9042426163613</v>
       </c>
       <c r="E5">
-        <v>-219.607915869027</v>
+        <v>-219.6078593919854</v>
       </c>
       <c r="F5">
-        <v>1.296385169700631</v>
+        <v>1.296383224375885</v>
       </c>
       <c r="G5">
-        <v>1.100000010651292</v>
+        <v>1.100000010873496</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2744,13 +2744,13 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>165.4281648001037</v>
+        <v>165.4281831740263</v>
       </c>
       <c r="E6">
-        <v>-164.8074848052748</v>
+        <v>-164.8075030949366</v>
       </c>
       <c r="F6">
-        <v>0.6206799948288211</v>
+        <v>0.6206800790897082</v>
       </c>
       <c r="G6">
         <v>1.02</v>

</xml_diff>

<commit_message>
Typos fixed in printout script of DCLF and DCOPF
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
   <si>
     <t>Conventional generation (MW)</t>
   </si>
@@ -40,16 +40,13 @@
     <t>angle(degs)</t>
   </si>
   <si>
-    <t>Voltage(p.u.)</t>
-  </si>
-  <si>
     <t>busname</t>
   </si>
   <si>
     <t>PD(MW)</t>
   </si>
   <si>
-    <t>QD(MVar)</t>
+    <t>alpha</t>
   </si>
   <si>
     <t>D1</t>
@@ -103,13 +100,13 @@
     <t>D9</t>
   </si>
   <si>
-    <t>PG(MW)</t>
+    <t>PGLB(MW)</t>
   </si>
   <si>
     <t>pG(MW)</t>
   </si>
   <si>
-    <t>qG(MVar)</t>
+    <t>PGUB(MW)</t>
   </si>
   <si>
     <t>G3</t>
@@ -217,13 +214,7 @@
     <t>to_busname</t>
   </si>
   <si>
-    <t>pLto(MW)</t>
-  </si>
-  <si>
-    <t>pLfrom(MW)</t>
-  </si>
-  <si>
-    <t>loss(MW)</t>
+    <t>pL(MW)</t>
   </si>
   <si>
     <t>L16-1223</t>
@@ -325,13 +316,7 @@
     <t>L28-1821</t>
   </si>
   <si>
-    <t>pLTto(MW)</t>
-  </si>
-  <si>
-    <t>pLTfrom(MW)</t>
-  </si>
-  <si>
-    <t>tap</t>
+    <t>pLT(MW)</t>
   </si>
   <si>
     <t>T2-911</t>
@@ -726,7 +711,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>2904.199958328551</v>
+        <v>2850.000028498455</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -735,7 +720,7 @@
         <v>2850</v>
       </c>
       <c r="D2">
-        <v>51.70103124997319</v>
+        <v>60998.39058603409</v>
       </c>
     </row>
   </sheetData>
@@ -745,285 +730,210 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-6.954336164209468</v>
-      </c>
-      <c r="C2">
-        <v>1.041171740726286</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>-132.6133918265722</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-6.987038895179992</v>
-      </c>
-      <c r="C3">
-        <v>1.035000000900278</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>-132.7051973714957</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-5.791314030672015</v>
-      </c>
-      <c r="C4">
-        <v>1.049999989553545</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>-132.1945556026775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-9.380426072626054</v>
-      </c>
-      <c r="C5">
-        <v>1.006629803587966</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>-135.9656598392043</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-9.703135100475894</v>
-      </c>
-      <c r="C6">
-        <v>1.023816162635372</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>-135.902402413119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-12.18984785700471</v>
-      </c>
-      <c r="C7">
-        <v>1.015735577424695</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>-138.6031151469106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-7.0138043603139</v>
-      </c>
-      <c r="C8">
-        <v>1.025000000861727</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>-139.267904099149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-10.7918773526312</v>
-      </c>
-      <c r="C9">
-        <v>0.996994344779235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>-140.8940238546722</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-7.255529263787974</v>
-      </c>
-      <c r="C10">
-        <v>1.016761895503189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>-134.2374831485872</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-9.343244474360933</v>
-      </c>
-      <c r="C11">
-        <v>1.032710967342917</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>-135.7472768271178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-2.175645845717776</v>
-      </c>
-      <c r="C12">
-        <v>0.993463264623684</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>-1.939599528520019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-1.519622106706469</v>
-      </c>
-      <c r="C13">
-        <v>1.007024443039843</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>-2.876568004860241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1.922255097482938e-22</v>
-      </c>
-      <c r="C14">
-        <v>1.020000000687559</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2.116497042707441</v>
-      </c>
-      <c r="C15">
-        <v>0.9800000029333509</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>1.897675616928149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10.47761840216531</v>
-      </c>
-      <c r="C16">
-        <v>1.09578684298166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>10.61277787743842</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>9.901490906490791</v>
-      </c>
-      <c r="C17">
-        <v>1.03552312332949</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>9.792611641984362</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>14.21567334744549</v>
-      </c>
-      <c r="C18">
-        <v>1.044723716059756</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>14.55364087426504</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>15.53637998996704</v>
-      </c>
-      <c r="C19">
-        <v>1.049999999808577</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>16.03803819224997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>8.557752832219609</v>
-      </c>
-      <c r="C20">
-        <v>1.033921973285685</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>8.411462625922606</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>9.284541911580224</v>
-      </c>
-      <c r="C21">
-        <v>1.042247791338515</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>9.280986778879916</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>16.29525361727388</v>
-      </c>
-      <c r="C22">
-        <v>1.050000356255982</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>16.87583811254465</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>21.98422090266471</v>
-      </c>
-      <c r="C23">
-        <v>1.050000000112305</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>23.05560240383218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>10.38975485847643</v>
-      </c>
-      <c r="C24">
-        <v>1.050000000393651</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>10.54732954440127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>4.964784838117613</v>
-      </c>
-      <c r="C25">
-        <v>1.027050270768929</v>
+        <v>4.266290769922725</v>
       </c>
     </row>
   </sheetData>
@@ -1044,18 +954,18 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1064,12 +974,12 @@
         <v>108</v>
       </c>
       <c r="D2">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1078,12 +988,12 @@
         <v>195</v>
       </c>
       <c r="D3">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>13</v>
@@ -1092,12 +1002,12 @@
         <v>265</v>
       </c>
       <c r="D4">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -1106,12 +1016,12 @@
         <v>194</v>
       </c>
       <c r="D5">
-        <v>39</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -1120,12 +1030,12 @@
         <v>317</v>
       </c>
       <c r="D6">
-        <v>64</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -1134,12 +1044,12 @@
         <v>100</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>18</v>
@@ -1148,12 +1058,12 @@
         <v>333</v>
       </c>
       <c r="D8">
-        <v>68</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>19</v>
@@ -1162,12 +1072,12 @@
         <v>181</v>
       </c>
       <c r="D9">
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1176,12 +1086,12 @@
         <v>97</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -1190,12 +1100,12 @@
         <v>128</v>
       </c>
       <c r="D11">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1204,12 +1114,12 @@
         <v>180</v>
       </c>
       <c r="D12">
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -1218,12 +1128,12 @@
         <v>74</v>
       </c>
       <c r="D13">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -1232,12 +1142,12 @@
         <v>71</v>
       </c>
       <c r="D14">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -1246,12 +1156,12 @@
         <v>136</v>
       </c>
       <c r="D15">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -1260,12 +1170,12 @@
         <v>125</v>
       </c>
       <c r="D16">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>8</v>
@@ -1274,12 +1184,12 @@
         <v>171</v>
       </c>
       <c r="D17">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>9</v>
@@ -1288,7 +1198,7 @@
         <v>175</v>
       </c>
       <c r="D18">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1309,16 +1219,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1326,16 +1236,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2">
-        <v>76</v>
+        <v>15.2</v>
       </c>
       <c r="D2">
         <v>76</v>
       </c>
       <c r="E2">
-        <v>10.469</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1343,16 +1253,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E3">
-        <v>10.469</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1360,16 +1270,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E4">
-        <v>10.469</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1377,16 +1287,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5">
-        <v>76</v>
+        <v>15.2</v>
       </c>
       <c r="D5">
         <v>76</v>
       </c>
       <c r="E5">
-        <v>10.469</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1394,16 +1304,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E6">
-        <v>-9.765000000000001</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1411,16 +1321,16 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>76</v>
+        <v>15.2</v>
       </c>
       <c r="D7">
         <v>76</v>
       </c>
       <c r="E7">
-        <v>-9.765000000000001</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1428,16 +1338,16 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E8">
-        <v>-9.765000000000001</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1445,16 +1355,16 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9">
-        <v>76</v>
+        <v>15.2</v>
       </c>
       <c r="D9">
         <v>76</v>
       </c>
       <c r="E9">
-        <v>-9.765000000000001</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1462,16 +1372,16 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>80</v>
+        <v>57.074</v>
       </c>
       <c r="E10">
-        <v>14.906</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1479,16 +1389,16 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>80</v>
+        <v>57.074</v>
       </c>
       <c r="E11">
-        <v>14.906</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1496,16 +1406,16 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>80</v>
+        <v>57.074</v>
       </c>
       <c r="E12">
-        <v>14.906</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1513,16 +1423,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>95.09999999999999</v>
+        <v>69</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>76.259</v>
       </c>
       <c r="E13">
-        <v>38.554</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1530,16 +1440,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14">
-        <v>95.09999999999999</v>
+        <v>69</v>
       </c>
       <c r="D14">
-        <v>95.09999999999999</v>
+        <v>76.259</v>
       </c>
       <c r="E14">
-        <v>38.554</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1547,16 +1457,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15">
-        <v>95.09999999999999</v>
+        <v>69</v>
       </c>
       <c r="D15">
-        <v>95.09999999999999</v>
+        <v>76.259</v>
       </c>
       <c r="E15">
-        <v>38.554</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1564,7 +1474,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1573,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>-85.18899999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1581,16 +1491,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17">
+        <v>2.4</v>
+      </c>
+      <c r="D17">
+        <v>2.4</v>
+      </c>
+      <c r="E17">
         <v>12</v>
-      </c>
-      <c r="D17">
-        <v>12</v>
-      </c>
-      <c r="E17">
-        <v>137.037</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1598,16 +1508,16 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18">
+        <v>2.4</v>
+      </c>
+      <c r="D18">
+        <v>2.4</v>
+      </c>
+      <c r="E18">
         <v>12</v>
-      </c>
-      <c r="D18">
-        <v>12</v>
-      </c>
-      <c r="E18">
-        <v>137.037</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1615,16 +1525,16 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19">
+        <v>2.4</v>
+      </c>
+      <c r="D19">
+        <v>2.4</v>
+      </c>
+      <c r="E19">
         <v>12</v>
-      </c>
-      <c r="D19">
-        <v>12</v>
-      </c>
-      <c r="E19">
-        <v>137.037</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1632,16 +1542,16 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20">
+        <v>2.4</v>
+      </c>
+      <c r="D20">
+        <v>2.4</v>
+      </c>
+      <c r="E20">
         <v>12</v>
-      </c>
-      <c r="D20">
-        <v>12</v>
-      </c>
-      <c r="E20">
-        <v>137.037</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1649,16 +1559,16 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21">
-        <v>155</v>
+        <v>54.3</v>
       </c>
       <c r="D21">
         <v>155</v>
       </c>
       <c r="E21">
-        <v>137.037</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1666,16 +1576,16 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22">
+        <v>2.4</v>
+      </c>
+      <c r="D22">
+        <v>2.4</v>
+      </c>
+      <c r="E22">
         <v>12</v>
-      </c>
-      <c r="D22">
-        <v>12</v>
-      </c>
-      <c r="E22">
-        <v>137.037</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1683,16 +1593,16 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23">
-        <v>155</v>
+        <v>54.3</v>
       </c>
       <c r="D23">
         <v>155</v>
       </c>
       <c r="E23">
-        <v>-204.612</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1700,16 +1610,16 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="D24">
         <v>400</v>
       </c>
       <c r="E24">
-        <v>93.45399999999999</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1717,16 +1627,16 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="D25">
         <v>400</v>
       </c>
       <c r="E25">
-        <v>-239.835</v>
+        <v>400</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1734,16 +1644,16 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D26">
         <v>50</v>
       </c>
       <c r="E26">
-        <v>-5.949</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1751,16 +1661,16 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <v>50</v>
       </c>
       <c r="E27">
-        <v>-5.949</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1768,16 +1678,16 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D28">
         <v>50</v>
       </c>
       <c r="E28">
-        <v>-5.949</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1785,16 +1695,16 @@
         <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>50</v>
       </c>
       <c r="E29">
-        <v>-5.949</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1802,16 +1712,16 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D30">
         <v>50</v>
       </c>
       <c r="E30">
-        <v>-5.949</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1819,16 +1729,16 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>50</v>
       </c>
       <c r="E31">
-        <v>-5.949</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1836,16 +1746,16 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32">
-        <v>155</v>
+        <v>54.3</v>
       </c>
       <c r="D32">
         <v>155</v>
       </c>
       <c r="E32">
-        <v>31.016</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1853,16 +1763,16 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33">
-        <v>350</v>
+        <v>140</v>
       </c>
       <c r="D33">
         <v>350</v>
       </c>
       <c r="E33">
-        <v>31.016</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1870,16 +1780,16 @@
         <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34">
-        <v>155</v>
+        <v>54.3</v>
       </c>
       <c r="D34">
         <v>155</v>
       </c>
       <c r="E34">
-        <v>31.016</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1900,16 +1810,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1919,35 +1829,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>68</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1956,18 +1860,12 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <v>231.0974088300875</v>
-      </c>
-      <c r="E2">
-        <v>-224.9052727344524</v>
-      </c>
-      <c r="F2">
-        <v>6.192136095635004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>-242.5374851810303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1976,18 +1874,12 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>-48.45925443476258</v>
-      </c>
-      <c r="E3">
-        <v>49.60070844371397</v>
-      </c>
-      <c r="F3">
-        <v>1.141454008951392</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>53.61358551709535</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -1996,18 +1888,12 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>177.8623638468168</v>
-      </c>
-      <c r="E4">
-        <v>-177.3404277294767</v>
-      </c>
-      <c r="F4">
-        <v>0.5219361173400383</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>-179.9140319902351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -2016,18 +1902,12 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>159.5927872348254</v>
-      </c>
-      <c r="E5">
-        <v>-157.5706497575499</v>
-      </c>
-      <c r="F5">
-        <v>2.022137477275576</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>-159.0814659002029</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -2036,18 +1916,12 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>369.3602581928429</v>
-      </c>
-      <c r="E6">
-        <v>-362.277622993714</v>
-      </c>
-      <c r="F6">
-        <v>7.082635199128884</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>-354.2226937566877</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -2056,18 +1930,12 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>-112.9343918605495</v>
-      </c>
-      <c r="E7">
-        <v>114.9999970027528</v>
-      </c>
-      <c r="F7">
-        <v>2.065605142203308</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>46.22336118165342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -2076,18 +1944,12 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>-28.30292709544883</v>
-      </c>
-      <c r="E8">
-        <v>28.67024434418971</v>
-      </c>
-      <c r="F8">
-        <v>0.3673172487408782</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>29.96286727379901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -2096,18 +1958,12 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>315.3324155686497</v>
-      </c>
-      <c r="E9">
-        <v>-312.323679657658</v>
-      </c>
-      <c r="F9">
-        <v>3.008735910991645</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>-320.8325709919405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2116,18 +1972,12 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>36.87525852921386</v>
-      </c>
-      <c r="E10">
-        <v>-36.52244851399961</v>
-      </c>
-      <c r="F10">
-        <v>0.3528100152142499</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>-29.08618448165901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>15</v>
@@ -2136,18 +1986,12 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <v>-220.9042426163613</v>
-      </c>
-      <c r="E11">
-        <v>224.6073084525962</v>
-      </c>
-      <c r="F11">
-        <v>3.703065836234876</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>213.4240769968072</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -2156,18 +2000,12 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <v>168.2776219955612</v>
-      </c>
-      <c r="E12">
-        <v>-166.5624347190722</v>
-      </c>
-      <c r="F12">
-        <v>1.715187276489027</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>-160.2226928064126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -2176,18 +2014,12 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>86.87483807478857</v>
-      </c>
-      <c r="E13">
-        <v>-86.30134756302856</v>
-      </c>
-      <c r="F13">
-        <v>0.5734905117600109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>-71.11848307296684</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2196,18 +2028,12 @@
         <v>23</v>
       </c>
       <c r="D14">
-        <v>226.8349498303853</v>
-      </c>
-      <c r="E14">
-        <v>-221.5777937823791</v>
-      </c>
-      <c r="F14">
-        <v>5.257156048006184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>-212.8157547310765</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -2216,18 +2042,12 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>101.0338173711477</v>
-      </c>
-      <c r="E15">
-        <v>-100.7580177567392</v>
-      </c>
-      <c r="F15">
-        <v>0.2757996144084673</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>-102.3233829498148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -2236,18 +2056,12 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <v>-110.0028256249187</v>
-      </c>
-      <c r="E16">
-        <v>112.7129099135157</v>
-      </c>
-      <c r="F16">
-        <v>2.710084288597092</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>82.74335966683338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -2256,18 +2070,12 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>140.4072067707107</v>
-      </c>
-      <c r="E17">
-        <v>-137.991987839173</v>
-      </c>
-      <c r="F17">
-        <v>2.41521893153771</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>-140.9185390017054</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2276,18 +2084,12 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>10.93761504779571</v>
-      </c>
-      <c r="E18">
-        <v>-10.87699104974649</v>
-      </c>
-      <c r="F18">
-        <v>0.06062399804922375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>-3.46120792309914</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -2296,18 +2098,12 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>55.52480781459366</v>
-      </c>
-      <c r="E19">
-        <v>-55.43118392294721</v>
-      </c>
-      <c r="F19">
-        <v>0.0936238916464438</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>-56.4570157609019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -2316,18 +2112,12 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>38.732361113112</v>
-      </c>
-      <c r="E20">
-        <v>-38.10815641637365</v>
-      </c>
-      <c r="F20">
-        <v>0.6242046967383508</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>-70.36859607155991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -2336,18 +2126,12 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>223.2605150646424</v>
-      </c>
-      <c r="E21">
-        <v>-219.6601124552858</v>
-      </c>
-      <c r="F21">
-        <v>3.600402609356612</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>-223.0837190883697</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -2356,18 +2140,12 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <v>88.57846656106835</v>
-      </c>
-      <c r="E22">
-        <v>-87.54074556523743</v>
-      </c>
-      <c r="F22">
-        <v>1.037720995830915</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>-82.38641584281369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2376,18 +2154,12 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>-37.47755148600039</v>
-      </c>
-      <c r="E23">
-        <v>37.97975438722105</v>
-      </c>
-      <c r="F23">
-        <v>0.5022029012206608</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>44.91381625825002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2396,18 +2168,12 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>-12.58046682726585</v>
-      </c>
-      <c r="E24">
-        <v>12.63044818795772</v>
-      </c>
-      <c r="F24">
-        <v>0.04998136069186976</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>11.52740309714622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B25">
         <v>19</v>
@@ -2416,18 +2182,12 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>36.75801775673923</v>
-      </c>
-      <c r="E25">
-        <v>-36.68037120899265</v>
-      </c>
-      <c r="F25">
-        <v>0.07764654774657376</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>-38.32338230986029</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B26">
         <v>20</v>
@@ -2436,18 +2196,12 @@
         <v>23</v>
       </c>
       <c r="D26">
-        <v>101.0338173711477</v>
-      </c>
-      <c r="E26">
-        <v>-100.7580177567392</v>
-      </c>
-      <c r="F26">
-        <v>0.2757996144084673</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>-102.3233829498148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2456,18 +2210,12 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <v>-61.45811387440724</v>
-      </c>
-      <c r="E27">
-        <v>62.24653886545782</v>
-      </c>
-      <c r="F27">
-        <v>0.7884249910505847</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>67.93380339415208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -2476,18 +2224,12 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>-107.6392575820147</v>
-      </c>
-      <c r="E28">
-        <v>107.9662455406568</v>
-      </c>
-      <c r="F28">
-        <v>0.326987958642122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>104.3532371901885</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -2496,18 +2238,12 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>20.2413939355046</v>
-      </c>
-      <c r="E29">
-        <v>-19.95745172307686</v>
-      </c>
-      <c r="F29">
-        <v>0.283942212427743</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>-54.40804445669571</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B30">
         <v>12</v>
@@ -2516,18 +2252,12 @@
         <v>13</v>
       </c>
       <c r="D30">
-        <v>59.90295271036039</v>
-      </c>
-      <c r="E30">
-        <v>-59.66698325979712</v>
-      </c>
-      <c r="F30">
-        <v>0.235969450563267</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>-105.4739135340946</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -2536,18 +2266,12 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>9.575011987546883</v>
-      </c>
-      <c r="E31">
-        <v>-9.541886125592757</v>
-      </c>
-      <c r="F31">
-        <v>0.03312586195412526</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>-3.066197315756954</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B32">
         <v>19</v>
@@ -2556,18 +2280,12 @@
         <v>20</v>
       </c>
       <c r="D32">
-        <v>36.75801775673923</v>
-      </c>
-      <c r="E32">
-        <v>-36.68037120899265</v>
-      </c>
-      <c r="F32">
-        <v>0.07764654774657376</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>-38.32338230986026</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B33">
         <v>15</v>
@@ -2576,18 +2294,12 @@
         <v>21</v>
       </c>
       <c r="D33">
-        <v>223.2605150646424</v>
-      </c>
-      <c r="E33">
-        <v>-219.6601124552858</v>
-      </c>
-      <c r="F33">
-        <v>3.600402609356612</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>-223.0837190883697</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B34">
         <v>18</v>
@@ -2596,13 +2308,7 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>55.52480781459366</v>
-      </c>
-      <c r="E34">
-        <v>-55.43118392294721</v>
-      </c>
-      <c r="F34">
-        <v>0.0936238916464438</v>
+        <v>-56.4570157609019</v>
       </c>
     </row>
   </sheetData>
@@ -2612,38 +2318,29 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -2652,21 +2349,12 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>103.751360831875</v>
-      </c>
-      <c r="E2">
-        <v>-103.498528788644</v>
-      </c>
-      <c r="F2">
-        <v>0.2528320432310105</v>
-      </c>
-      <c r="G2">
-        <v>1.03</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>-89.20351550662039</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -2675,21 +2363,12 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>119.1440728202233</v>
-      </c>
-      <c r="E3">
-        <v>-118.8061637582331</v>
-      </c>
-      <c r="F3">
-        <v>0.3379090619902048</v>
-      </c>
-      <c r="G3">
-        <v>1.03</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>-155.2883995227085</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -2698,21 +2377,12 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>149.1124214502258</v>
-      </c>
-      <c r="E4">
-        <v>-148.5873693891832</v>
-      </c>
-      <c r="F4">
-        <v>0.5250520610425191</v>
-      </c>
-      <c r="G4">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>-142.137660372759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2721,21 +2391,12 @@
         <v>24</v>
       </c>
       <c r="D5">
-        <v>220.9042426163613</v>
-      </c>
-      <c r="E5">
-        <v>-219.6078593919854</v>
-      </c>
-      <c r="F5">
-        <v>1.296383224375885</v>
-      </c>
-      <c r="G5">
-        <v>1.100000010873496</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>-213.4240769968072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -2744,16 +2405,7 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>165.4281831740263</v>
-      </c>
-      <c r="E6">
-        <v>-164.8075030949366</v>
-      </c>
-      <c r="F6">
-        <v>0.6206800790897082</v>
-      </c>
-      <c r="G6">
-        <v>1.02</v>
+        <v>-192.7229991924163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some minor output issues fixed
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
   <si>
     <t>Conventional generation (MW)</t>
   </si>
@@ -40,12 +40,18 @@
     <t>angle(degs)</t>
   </si>
   <si>
+    <t>Voltage(p.u.)</t>
+  </si>
+  <si>
     <t>busname</t>
   </si>
   <si>
     <t>PD(MW)</t>
   </si>
   <si>
+    <t>QD(MVar)</t>
+  </si>
+  <si>
     <t>alpha</t>
   </si>
   <si>
@@ -103,12 +109,24 @@
     <t>PGLB(MW)</t>
   </si>
   <si>
+    <t>PG(MW)</t>
+  </si>
+  <si>
     <t>pG(MW)</t>
   </si>
   <si>
     <t>PGUB(MW)</t>
   </si>
   <si>
+    <t>QGLB(MVar)</t>
+  </si>
+  <si>
+    <t>qG(MVar)</t>
+  </si>
+  <si>
+    <t>QGUB(MVar)</t>
+  </si>
+  <si>
     <t>G3</t>
   </si>
   <si>
@@ -214,7 +232,13 @@
     <t>to_busname</t>
   </si>
   <si>
-    <t>pL(MW)</t>
+    <t>pLto(MW)</t>
+  </si>
+  <si>
+    <t>pLfrom(MW)</t>
+  </si>
+  <si>
+    <t>loss(MW)</t>
   </si>
   <si>
     <t>L16-1223</t>
@@ -316,7 +340,10 @@
     <t>L28-1821</t>
   </si>
   <si>
-    <t>pLT(MW)</t>
+    <t>pLTto(MW)</t>
+  </si>
+  <si>
+    <t>pLTfrom(MW)</t>
   </si>
   <si>
     <t>T2-911</t>
@@ -711,7 +738,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>2850.000028498455</v>
+        <v>2896.357344121534</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -720,7 +747,7 @@
         <v>2850</v>
       </c>
       <c r="D2">
-        <v>60998.39058603409</v>
+        <v>3805.990532205099</v>
       </c>
     </row>
   </sheetData>
@@ -730,210 +757,285 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-132.6133918265722</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>-6.466152699262157</v>
+      </c>
+      <c r="C2">
+        <v>1.049999982605085</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-132.7051973714957</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>-6.539232816460347</v>
+      </c>
+      <c r="C3">
+        <v>1.049999979600153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-132.1945556026775</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>-6.03888140370221</v>
+      </c>
+      <c r="C4">
+        <v>1.024290155903114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-135.9656598392043</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>-9.299110087850506</v>
+      </c>
+      <c r="C5">
+        <v>1.02461465963264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-135.902402413119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>-9.423394686507905</v>
+      </c>
+      <c r="C6">
+        <v>1.036874229239571</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-138.6031151469106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>-11.98517030355955</v>
+      </c>
+      <c r="C7">
+        <v>1.033109845798978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-139.267904099149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>-9.178634767023798</v>
+      </c>
+      <c r="C8">
+        <v>1.049558580161324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-140.8940238546722</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>-11.97422891942581</v>
+      </c>
+      <c r="C9">
+        <v>1.019821468140645</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-134.2374831485872</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>-7.616014636592167</v>
+      </c>
+      <c r="C10">
+        <v>1.036522608195682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-135.7472768271178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>-9.350744214096236</v>
+      </c>
+      <c r="C11">
+        <v>1.050000003759179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-1.939599528520019</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>-2.489563043343162</v>
+      </c>
+      <c r="C12">
+        <v>1.029169240451002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-2.876568004860241</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>-1.779390337709839</v>
+      </c>
+      <c r="C13">
+        <v>1.02382200581327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>-1.084761611808807e-27</v>
+      </c>
+      <c r="C14">
+        <v>1.041088371710202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1.897675616928149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>1.100610516668815</v>
+      </c>
+      <c r="C15">
+        <v>1.045304584495609</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10.61277787743842</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>9.40082914351291</v>
+      </c>
+      <c r="C16">
+        <v>1.041756176226173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>9.792611641984362</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>8.608974567893155</v>
+      </c>
+      <c r="C17">
+        <v>1.045677551223554</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>14.55364087426504</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>12.9603964889255</v>
+      </c>
+      <c r="C18">
+        <v>1.048020674380289</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>16.03803819224997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>14.31984170322459</v>
+      </c>
+      <c r="C19">
+        <v>1.049999996444465</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>8.411462625922606</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>7.55353488691155</v>
+      </c>
+      <c r="C20">
+        <v>1.039754074509631</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>9.280986778879916</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>8.504587797921708</v>
+      </c>
+      <c r="C21">
+        <v>1.044261765460458</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>16.87583811254465</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>15.09713696277908</v>
+      </c>
+      <c r="C22">
+        <v>1.050000005527165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>23.05560240383218</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>20.76316616302879</v>
+      </c>
+      <c r="C23">
+        <v>1.050000002059877</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>10.54732954440127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>9.731913424459648</v>
+      </c>
+      <c r="C24">
+        <v>1.050000005217705</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>4.266290769922725</v>
+        <v>3.781897527061615</v>
+      </c>
+      <c r="C25">
+        <v>1.005838071555074</v>
       </c>
     </row>
   </sheetData>
@@ -943,272 +1045,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>108</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>195</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>265</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>194</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>317</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>16</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>333</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>181</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>97</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>20</v>
-      </c>
-      <c r="C11">
-        <v>128</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>180</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>74</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>71</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>136</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>125</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>171</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>175</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1219,24 +1056,355 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>108</v>
+      </c>
+      <c r="D2">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>195</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>265</v>
+      </c>
+      <c r="D4">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>194</v>
+      </c>
+      <c r="D5">
+        <v>39</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>317</v>
+      </c>
+      <c r="D6">
+        <v>64</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>333</v>
+      </c>
+      <c r="D8">
+        <v>68</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>181</v>
+      </c>
+      <c r="D9">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>97</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>128</v>
+      </c>
+      <c r="D11">
+        <v>26</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>180</v>
+      </c>
+      <c r="D12">
+        <v>37</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>74</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>71</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
         <v>6</v>
       </c>
+      <c r="C15">
+        <v>136</v>
+      </c>
+      <c r="D15">
+        <v>28</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>125</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>171</v>
+      </c>
+      <c r="D17">
+        <v>35</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>175</v>
+      </c>
+      <c r="D18">
+        <v>36</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>15.2</v>
@@ -1247,13 +1415,25 @@
       <c r="E2">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>76</v>
+      </c>
+      <c r="G2">
+        <v>-25</v>
+      </c>
+      <c r="H2">
+        <v>-2.778</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -1262,15 +1442,27 @@
         <v>16</v>
       </c>
       <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>4.819</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -1279,15 +1471,27 @@
         <v>16</v>
       </c>
       <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>4.819</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>15.2</v>
@@ -1298,13 +1502,25 @@
       <c r="E5">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>76</v>
+      </c>
+      <c r="G5">
+        <v>-25</v>
+      </c>
+      <c r="H5">
+        <v>-2.778</v>
+      </c>
+      <c r="I5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -1313,15 +1529,27 @@
         <v>16</v>
       </c>
       <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>4.751</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>15.2</v>
@@ -1332,13 +1560,25 @@
       <c r="E7">
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>76</v>
+      </c>
+      <c r="G7">
+        <v>-25</v>
+      </c>
+      <c r="H7">
+        <v>-4.543</v>
+      </c>
+      <c r="I7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1347,15 +1587,27 @@
         <v>16</v>
       </c>
       <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>4.751</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>15.2</v>
@@ -1366,115 +1618,199 @@
       <c r="E9">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>76</v>
+      </c>
+      <c r="G9">
+        <v>-25</v>
+      </c>
+      <c r="H9">
+        <v>-4.543</v>
+      </c>
+      <c r="I9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>25</v>
       </c>
       <c r="D10">
-        <v>57.074</v>
+        <v>57.054</v>
       </c>
       <c r="E10">
+        <v>72.50700000000001</v>
+      </c>
+      <c r="F10">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>17.678</v>
+      </c>
+      <c r="I10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C11">
         <v>25</v>
       </c>
       <c r="D11">
-        <v>57.074</v>
+        <v>57.054</v>
       </c>
       <c r="E11">
+        <v>72.50700000000001</v>
+      </c>
+      <c r="F11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>17.678</v>
+      </c>
+      <c r="I11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C12">
         <v>25</v>
       </c>
       <c r="D12">
-        <v>57.074</v>
+        <v>57.054</v>
       </c>
       <c r="E12">
+        <v>72.50700000000001</v>
+      </c>
+      <c r="F12">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>17.678</v>
+      </c>
+      <c r="I12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>69</v>
       </c>
       <c r="D13">
-        <v>76.259</v>
+        <v>76.279</v>
       </c>
       <c r="E13">
+        <v>76.279</v>
+      </c>
+      <c r="F13">
         <v>197</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>37.496</v>
+      </c>
+      <c r="I13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C14">
         <v>69</v>
       </c>
       <c r="D14">
-        <v>76.259</v>
+        <v>76.279</v>
       </c>
       <c r="E14">
+        <v>76.279</v>
+      </c>
+      <c r="F14">
         <v>197</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>37.496</v>
+      </c>
+      <c r="I14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C15">
         <v>69</v>
       </c>
       <c r="D15">
-        <v>76.259</v>
+        <v>76.279</v>
       </c>
       <c r="E15">
+        <v>76.279</v>
+      </c>
+      <c r="F15">
         <v>197</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>37.496</v>
+      </c>
+      <c r="I15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1485,13 +1821,25 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>-50</v>
+      </c>
+      <c r="H16">
+        <v>123.049</v>
+      </c>
+      <c r="I16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C17">
         <v>2.4</v>
@@ -1500,15 +1848,27 @@
         <v>2.4</v>
       </c>
       <c r="E17">
+        <v>2.4</v>
+      </c>
+      <c r="F17">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <v>2.4</v>
@@ -1517,15 +1877,27 @@
         <v>2.4</v>
       </c>
       <c r="E18">
+        <v>2.4</v>
+      </c>
+      <c r="F18">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C19">
         <v>2.4</v>
@@ -1534,15 +1906,27 @@
         <v>2.4</v>
       </c>
       <c r="E19">
+        <v>2.4</v>
+      </c>
+      <c r="F19">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C20">
         <v>2.4</v>
@@ -1551,15 +1935,27 @@
         <v>2.4</v>
       </c>
       <c r="E20">
+        <v>2.4</v>
+      </c>
+      <c r="F20">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C21">
         <v>54.3</v>
@@ -1570,13 +1966,25 @@
       <c r="E21">
         <v>155</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <v>155</v>
+      </c>
+      <c r="G21">
+        <v>-50</v>
+      </c>
+      <c r="H21">
+        <v>80</v>
+      </c>
+      <c r="I21">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>2.4</v>
@@ -1585,15 +1993,27 @@
         <v>2.4</v>
       </c>
       <c r="E22">
+        <v>2.4</v>
+      </c>
+      <c r="F22">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+      <c r="I22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C23">
         <v>54.3</v>
@@ -1604,13 +2024,25 @@
       <c r="E23">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <v>155</v>
+      </c>
+      <c r="G23">
+        <v>-50</v>
+      </c>
+      <c r="H23">
+        <v>80</v>
+      </c>
+      <c r="I23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C24">
         <v>100</v>
@@ -1621,13 +2053,25 @@
       <c r="E24">
         <v>400</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <v>400</v>
+      </c>
+      <c r="G24">
+        <v>-50</v>
+      </c>
+      <c r="H24">
+        <v>69.587</v>
+      </c>
+      <c r="I24">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C25">
         <v>100</v>
@@ -1638,13 +2082,25 @@
       <c r="E25">
         <v>400</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <v>400</v>
+      </c>
+      <c r="G25">
+        <v>-50</v>
+      </c>
+      <c r="H25">
+        <v>-10.445</v>
+      </c>
+      <c r="I25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -1655,13 +2111,25 @@
       <c r="E26">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26">
+        <v>-10</v>
+      </c>
+      <c r="H26">
+        <v>-6.488</v>
+      </c>
+      <c r="I26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -1672,13 +2140,25 @@
       <c r="E27">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>50</v>
+      </c>
+      <c r="G27">
+        <v>-10</v>
+      </c>
+      <c r="H27">
+        <v>-6.488</v>
+      </c>
+      <c r="I27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -1689,13 +2169,25 @@
       <c r="E28">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>-10</v>
+      </c>
+      <c r="H28">
+        <v>-6.488</v>
+      </c>
+      <c r="I28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -1706,13 +2198,25 @@
       <c r="E29">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <v>50</v>
+      </c>
+      <c r="G29">
+        <v>-10</v>
+      </c>
+      <c r="H29">
+        <v>-6.488</v>
+      </c>
+      <c r="I29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C30">
         <v>10</v>
@@ -1723,13 +2227,25 @@
       <c r="E30">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>-10</v>
+      </c>
+      <c r="H30">
+        <v>-6.488</v>
+      </c>
+      <c r="I30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -1740,13 +2256,25 @@
       <c r="E31">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31">
+        <v>-10</v>
+      </c>
+      <c r="H31">
+        <v>-6.488</v>
+      </c>
+      <c r="I31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C32">
         <v>54.3</v>
@@ -1757,13 +2285,25 @@
       <c r="E32">
         <v>155</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <v>155</v>
+      </c>
+      <c r="G32">
+        <v>-50</v>
+      </c>
+      <c r="H32">
+        <v>-2.675</v>
+      </c>
+      <c r="I32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C33">
         <v>140</v>
@@ -1774,13 +2314,25 @@
       <c r="E33">
         <v>350</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <v>350</v>
+      </c>
+      <c r="G33">
+        <v>-25</v>
+      </c>
+      <c r="H33">
+        <v>32.09</v>
+      </c>
+      <c r="I33">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C34">
         <v>54.3</v>
@@ -1790,6 +2342,18 @@
       </c>
       <c r="E34">
         <v>155</v>
+      </c>
+      <c r="F34">
+        <v>155</v>
+      </c>
+      <c r="G34">
+        <v>-50</v>
+      </c>
+      <c r="H34">
+        <v>-2.675</v>
+      </c>
+      <c r="I34">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1799,27 +2363,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1829,29 +2402,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>70</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1860,12 +2439,18 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <v>-242.5374851810303</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>224.9018551391359</v>
+      </c>
+      <c r="E2">
+        <v>-219.1586582294877</v>
+      </c>
+      <c r="F2">
+        <v>5.74319690964824</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1874,12 +2459,18 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>53.61358551709535</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>-51.83931743099927</v>
+      </c>
+      <c r="E3">
+        <v>53.11272326775494</v>
+      </c>
+      <c r="F3">
+        <v>1.27340583675567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -1888,12 +2479,18 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>-179.9140319902351</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>180.5506535287781</v>
+      </c>
+      <c r="E4">
+        <v>-180.0178475993984</v>
+      </c>
+      <c r="F4">
+        <v>0.5328059293797427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -1902,12 +2499,18 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>-159.0814659002029</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>158.9473565951548</v>
+      </c>
+      <c r="E5">
+        <v>-156.9414802812995</v>
+      </c>
+      <c r="F5">
+        <v>2.005876313855315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -1916,12 +2519,18 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>-354.2226937566877</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>364.3780295063975</v>
+      </c>
+      <c r="E6">
+        <v>-358.2851580490458</v>
+      </c>
+      <c r="F6">
+        <v>6.092871457351734</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1930,12 +2539,18 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>46.22336118165342</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>-91.16378300843239</v>
+      </c>
+      <c r="E7">
+        <v>92.5202780260517</v>
+      </c>
+      <c r="F7">
+        <v>1.356495017619308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1944,12 +2559,18 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>29.96286727379901</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>-20.34709303102877</v>
+      </c>
+      <c r="E8">
+        <v>20.54156397175313</v>
+      </c>
+      <c r="F8">
+        <v>0.19447094072437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -1958,12 +2579,18 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>-320.8325709919405</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>318.6291958931679</v>
+      </c>
+      <c r="E9">
+        <v>-315.5681215135626</v>
+      </c>
+      <c r="F9">
+        <v>3.061074379605344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1972,12 +2599,18 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>-29.08618448165901</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>31.18765452638066</v>
+      </c>
+      <c r="E10">
+        <v>-30.94044702405075</v>
+      </c>
+      <c r="F10">
+        <v>0.2472075023299047</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B11">
         <v>15</v>
@@ -1986,12 +2619,18 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <v>213.4240769968072</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>-202.0462707815688</v>
+      </c>
+      <c r="E11">
+        <v>204.8255093261738</v>
+      </c>
+      <c r="F11">
+        <v>2.779238544604956</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -2000,12 +2639,18 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <v>-160.2226928064126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>164.2851566655688</v>
+      </c>
+      <c r="E12">
+        <v>-162.9224246835644</v>
+      </c>
+      <c r="F12">
+        <v>1.362731982004406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -2014,12 +2659,18 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>-71.11848307296684</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>99.7506439782118</v>
+      </c>
+      <c r="E13">
+        <v>-99.17728101756124</v>
+      </c>
+      <c r="F13">
+        <v>0.5733629606505586</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2028,12 +2679,18 @@
         <v>23</v>
       </c>
       <c r="D14">
-        <v>-212.8157547310765</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>213.8229066190032</v>
+      </c>
+      <c r="E14">
+        <v>-209.219534316267</v>
+      </c>
+      <c r="F14">
+        <v>4.603372302736242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -2042,12 +2699,18 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>-102.3233829498148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>110.6376195635052</v>
+      </c>
+      <c r="E15">
+        <v>-110.3212444579575</v>
+      </c>
+      <c r="F15">
+        <v>0.3163751055476727</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -2056,12 +2719,18 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <v>82.74335966683338</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>-82.59520317011139</v>
+      </c>
+      <c r="E16">
+        <v>82.75683685031591</v>
+      </c>
+      <c r="F16">
+        <v>0.1616336802045204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -2070,12 +2739,18 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>-140.9185390017054</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>141.052644027376</v>
+      </c>
+      <c r="E17">
+        <v>-138.6113482937696</v>
+      </c>
+      <c r="F17">
+        <v>2.44129573360643</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2084,12 +2759,18 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>-3.46120792309914</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>0.5414575520811779</v>
+      </c>
+      <c r="E18">
+        <v>-0.4587536960814427</v>
+      </c>
+      <c r="F18">
+        <v>0.08270385599973519</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -2098,12 +2779,18 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>-56.4570157609019</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>56.87355281830472</v>
+      </c>
+      <c r="E19">
+        <v>-56.77532842446865</v>
+      </c>
+      <c r="F19">
+        <v>0.09822439383606607</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -2112,12 +2799,18 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>-70.36859607155991</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>48.59461563902457</v>
+      </c>
+      <c r="E20">
+        <v>-47.65606766631542</v>
+      </c>
+      <c r="F20">
+        <v>0.9385479727091528</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -2126,12 +2819,18 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <v>-223.0837190883697</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>221.5971873223451</v>
+      </c>
+      <c r="E21">
+        <v>-218.7911672099672</v>
+      </c>
+      <c r="F21">
+        <v>2.806020112377849</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -2140,12 +2839,18 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <v>-82.38641584281369</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>85.09067244310276</v>
+      </c>
+      <c r="E22">
+        <v>-84.16068391906867</v>
+      </c>
+      <c r="F22">
+        <v>0.9299885240340866</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2154,12 +2859,18 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>44.91381625825002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>-43.05955370602915</v>
+      </c>
+      <c r="E23">
+        <v>43.66086635803253</v>
+      </c>
+      <c r="F23">
+        <v>0.6013126520033829</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2168,12 +2879,18 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>11.52740309714622</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>-9.773573722580853</v>
+      </c>
+      <c r="E24">
+        <v>9.775905785322495</v>
+      </c>
+      <c r="F24">
+        <v>0.002332062741641772</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B25">
         <v>19</v>
@@ -2182,12 +2899,18 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>-38.32338230986029</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>46.32124382288884</v>
+      </c>
+      <c r="E25">
+        <v>-46.21903945871017</v>
+      </c>
+      <c r="F25">
+        <v>0.1022043641786652</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B26">
         <v>20</v>
@@ -2196,12 +2919,18 @@
         <v>23</v>
       </c>
       <c r="D26">
-        <v>-102.3233829498148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>110.6376195635052</v>
+      </c>
+      <c r="E26">
+        <v>-110.3212444579575</v>
+      </c>
+      <c r="F26">
+        <v>0.3163751055476727</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2210,12 +2939,18 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <v>67.93380339415208</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>-65.80349172816798</v>
+      </c>
+      <c r="E27">
+        <v>66.68286337335645</v>
+      </c>
+      <c r="F27">
+        <v>0.8793716451884759</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -2224,12 +2959,18 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>104.3532371901885</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>-88.56192288271316</v>
+      </c>
+      <c r="E28">
+        <v>88.78529450533583</v>
+      </c>
+      <c r="F28">
+        <v>0.2233716226226701</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -2238,12 +2979,18 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>-54.40804445669571</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>32.64345730532149</v>
+      </c>
+      <c r="E29">
+        <v>-32.18015102531122</v>
+      </c>
+      <c r="F29">
+        <v>0.4633062800102783</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B30">
         <v>12</v>
@@ -2252,12 +2999,18 @@
         <v>13</v>
       </c>
       <c r="D30">
-        <v>-105.4739135340946</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>73.30590186812178</v>
+      </c>
+      <c r="E30">
+        <v>-72.95465517313622</v>
+      </c>
+      <c r="F30">
+        <v>0.351246694985563</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -2266,12 +3019,18 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>-3.066197315756954</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>5.244220389979626</v>
+      </c>
+      <c r="E31">
+        <v>-5.196508971917122</v>
+      </c>
+      <c r="F31">
+        <v>0.04771141806250295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B32">
         <v>19</v>
@@ -2280,12 +3039,18 @@
         <v>20</v>
       </c>
       <c r="D32">
-        <v>-38.32338230986026</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>46.32124382288884</v>
+      </c>
+      <c r="E32">
+        <v>-46.21903945871017</v>
+      </c>
+      <c r="F32">
+        <v>0.1022043641786652</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B33">
         <v>15</v>
@@ -2294,12 +3059,18 @@
         <v>21</v>
       </c>
       <c r="D33">
-        <v>-223.0837190883697</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>221.5971873223451</v>
+      </c>
+      <c r="E33">
+        <v>-218.7911672099672</v>
+      </c>
+      <c r="F33">
+        <v>2.806020112377849</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B34">
         <v>18</v>
@@ -2308,7 +3079,13 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>-56.4570157609019</v>
+        <v>56.87355281830472</v>
+      </c>
+      <c r="E34">
+        <v>-56.77532842446865</v>
+      </c>
+      <c r="F34">
+        <v>0.09822439383606607</v>
       </c>
     </row>
   </sheetData>
@@ -2318,29 +3095,35 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>106</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -2349,12 +3132,18 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>-89.20351550662039</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>111.1211820896329</v>
+      </c>
+      <c r="E2">
+        <v>-110.833631647682</v>
+      </c>
+      <c r="F2">
+        <v>0.2875504419509456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -2363,12 +3152,18 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>-155.2883995227085</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>123.9836595110117</v>
+      </c>
+      <c r="E3">
+        <v>-123.6015472267869</v>
+      </c>
+      <c r="F3">
+        <v>0.3821122842248226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -2377,12 +3172,18 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>-142.137660372759</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>150.9785236114927</v>
+      </c>
+      <c r="E4">
+        <v>-150.4830862715429</v>
+      </c>
+      <c r="F4">
+        <v>0.4954373399498335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2391,12 +3192,18 @@
         <v>24</v>
       </c>
       <c r="D5">
-        <v>-213.4240769968072</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>202.0462707815688</v>
+      </c>
+      <c r="E5">
+        <v>-201.0830233139372</v>
+      </c>
+      <c r="F5">
+        <v>0.9632474676316338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -2405,7 +3212,13 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>-192.7229991924163</v>
+        <v>168.1296538916122</v>
+      </c>
+      <c r="E6">
+        <v>-167.4952658069498</v>
+      </c>
+      <c r="F6">
+        <v>0.6343880846623851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>